<commit_message>
Ref 6 Formatted and added parts to the BOM.
</commit_message>
<xml_diff>
--- a/LegacyIOBoardBOM.xlsx
+++ b/LegacyIOBoardBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aasleso\Documents\New-Hydra-Legacy-IO-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0316705F-96C5-4760-AD65-66709E447AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D38281-E81B-4D9A-A841-7D342EC4D6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{E75E0199-A4FC-4142-9D32-2C5EB3346CD5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
   <si>
     <t>Reference</t>
   </si>
@@ -31,21 +31,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>DNP</t>
-  </si>
-  <si>
-    <t>Exclude from BOM</t>
-  </si>
-  <si>
-    <t>Exclude from Board</t>
-  </si>
-  <si>
-    <t>Footprint</t>
-  </si>
-  <si>
-    <t>Datasheet</t>
-  </si>
-  <si>
     <t>C1,C12</t>
   </si>
   <si>
@@ -82,111 +67,30 @@
     <t>D1,D5,D13,D14,D16,D17,D21,D22,D23,D24,D25</t>
   </si>
   <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>D3,D4,D6,D7,D8,D9,D10,D11,D12,D15</t>
-  </si>
-  <si>
-    <t>BAS16LT3G</t>
-  </si>
-  <si>
-    <t>BAS16LT3G:SOT95P240X111-3N</t>
-  </si>
-  <si>
-    <t>D18</t>
-  </si>
-  <si>
-    <t>1N4148WT</t>
-  </si>
-  <si>
-    <t>Diode_SMD:D_SOD-523</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/ds30396.pdf</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
-    <t>350826-1</t>
-  </si>
-  <si>
-    <t>CONN_350826-1_TYC</t>
-  </si>
-  <si>
-    <t>J2,J6,J24,J28</t>
-  </si>
-  <si>
-    <t>A_In</t>
-  </si>
-  <si>
-    <t>J3,J7,J25,J29</t>
-  </si>
-  <si>
-    <t>A_Out</t>
-  </si>
-  <si>
     <t>J4,J5,J8,J9,J22,J23,J26,J27</t>
   </si>
   <si>
-    <t>CONN_67800-5005_MOL</t>
-  </si>
-  <si>
     <t>J10,J11,J12,J13</t>
   </si>
   <si>
-    <t>AFBR-59R5LZ</t>
-  </si>
-  <si>
-    <t>AFBR59R5LZ</t>
-  </si>
-  <si>
-    <t>http://www.avagotech.com/pages/en/optical_transceivers/storage/4g_fibre_channel/afbr-59r5lz/</t>
-  </si>
-  <si>
     <t>J14,J15,J16,J17,J18,J19,J20,J21</t>
   </si>
   <si>
-    <t>CONN_SDA_42002-xxxxx_03_MOL</t>
-  </si>
-  <si>
     <t>J31</t>
   </si>
   <si>
-    <t>B08B-PASKLFSN</t>
-  </si>
-  <si>
-    <t>CONN_B08B-PASK_JST</t>
-  </si>
-  <si>
     <t>K1,K2,K3,K10</t>
   </si>
   <si>
-    <t>PR23-12V-900-1C</t>
-  </si>
-  <si>
-    <t>PR23-12V-900-1C:RELAY_PR23-12V-900-1C</t>
-  </si>
-  <si>
     <t>K4,K5,K6,K7</t>
   </si>
   <si>
-    <t>HE722A1200</t>
-  </si>
-  <si>
-    <t>HE722_LTF</t>
-  </si>
-  <si>
     <t>K9,K11</t>
   </si>
   <si>
-    <t>G5LE-1-VD-DC12</t>
-  </si>
-  <si>
-    <t>G5LE-1_OMR</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -247,50 +151,125 @@
     <t>AP62300TWU-7</t>
   </si>
   <si>
-    <t>TSOT26-WU_DIO</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
-    <t>SC0192_9_</t>
-  </si>
-  <si>
-    <t>SC0192_9_:MODULE_SC0192_9_</t>
-  </si>
-  <si>
     <t>U4,U5,U6,U7,U8,U10,U11,U13,U15,U17</t>
   </si>
   <si>
     <t>DMN3023L-7</t>
   </si>
   <si>
-    <t>SOT-23_2P9X1P3_DIO</t>
-  </si>
-  <si>
     <t>U9,U12,U14,U16</t>
   </si>
   <si>
-    <t>SFH615A-4X009</t>
-  </si>
-  <si>
-    <t>SFH615A-4X009:SOIC254P1016X390-4N</t>
-  </si>
-  <si>
     <t>U18</t>
   </si>
   <si>
     <t>AP3211KTR-G1</t>
   </si>
   <si>
-    <t>SOT23-6_DIO</t>
+    <t>Supplier Part Number</t>
+  </si>
+  <si>
+    <t>732-4982-1-ND</t>
+  </si>
+  <si>
+    <t>Line Item</t>
+  </si>
+  <si>
+    <t>BAS16LT3GOSCT-ND</t>
+  </si>
+  <si>
+    <t>D3,D4,D6,D7,D8,D9,D10,D11,D12,D15,D18</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>A14329-ND</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>J2,J3,J6,J7,J24,J25,J28,J29</t>
+  </si>
+  <si>
+    <t>AE10399-ND</t>
+  </si>
+  <si>
+    <t>J-1522</t>
+  </si>
+  <si>
+    <t>HE108-ND</t>
+  </si>
+  <si>
+    <t>2223-PR23-12V-900-1C-ND</t>
+  </si>
+  <si>
+    <t>39-G5LE-1-VDDC12-ND</t>
+  </si>
+  <si>
+    <t>SFH615A-4X009-ND</t>
+  </si>
+  <si>
+    <t>WM13101-ND</t>
+  </si>
+  <si>
+    <t>455-1823-ND</t>
+  </si>
+  <si>
+    <t>Pi4</t>
+  </si>
+  <si>
+    <t>A-4193538</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>Daktronics</t>
+  </si>
+  <si>
+    <t>311-0.0ARCT-ND</t>
+  </si>
+  <si>
+    <t>311-10.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t>311-1.00KCRCT-ND</t>
+  </si>
+  <si>
+    <t>Jumper resistors</t>
+  </si>
+  <si>
+    <t>P56.2KHTR-ND</t>
+  </si>
+  <si>
+    <t>13-RT1206DRE079KLTR-ND</t>
+  </si>
+  <si>
+    <t>P49.9KDCTR-ND</t>
+  </si>
+  <si>
+    <t>311-243LRTR-ND</t>
+  </si>
+  <si>
+    <t>311-16.2KHRTR-ND</t>
+  </si>
+  <si>
+    <t>CL21A106KOQNNNG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,8 +404,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -604,6 +591,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -723,7 +716,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -766,11 +759,38 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -804,6 +824,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1144,533 +1165,683 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6FEE036-4CF9-483C-8C65-E8C9586B780D}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="86.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="2">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="2">
         <v>8</v>
       </c>
-      <c r="B2">
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="D17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="2">
+        <v>11</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>25</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="3">
+        <v>32</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="2">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2">
+        <v>244</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
+      <c r="D30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="2">
+        <v>4</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="2">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
-      </c>
-      <c r="C13">
-        <v>678005005</v>
-      </c>
-      <c r="G13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13">
-        <v>678005005</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15">
-        <v>8</v>
-      </c>
-      <c r="C15">
-        <v>10845031</v>
-      </c>
-      <c r="G15" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15">
-        <v>10845031</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22">
-        <v>12</v>
-      </c>
-      <c r="C22" t="s">
-        <v>60</v>
-      </c>
-      <c r="H22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24">
-        <v>11</v>
-      </c>
-      <c r="C24" t="s">
-        <v>64</v>
-      </c>
-      <c r="H24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>66</v>
-      </c>
-      <c r="H25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26">
-        <v>32</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="H26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>69</v>
-      </c>
-      <c r="H27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28">
-        <v>4</v>
-      </c>
-      <c r="C28">
-        <v>244</v>
-      </c>
-      <c r="H28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>72</v>
-      </c>
-      <c r="H29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>74</v>
-      </c>
-      <c r="G30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>77</v>
-      </c>
-      <c r="G31" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32">
-        <v>10</v>
-      </c>
-      <c r="C32" t="s">
-        <v>80</v>
-      </c>
-      <c r="G32" t="s">
-        <v>81</v>
-      </c>
-      <c r="H32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
-        <v>83</v>
-      </c>
-      <c r="G33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>86</v>
-      </c>
-      <c r="G34" t="s">
-        <v>87</v>
-      </c>
-      <c r="H34" t="s">
-        <v>86</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150080BS75000/732-4982-1-ND/4489910" xr:uid="{F28DB25A-81E7-42A4-91EF-90BD6F9ECF00}"/>
+    <hyperlink ref="F8" r:id="rId2" display="https://www.digikey.com/product-detail/en/on-semiconductor/BAS16LT3G/BAS16LT3GOSCT-ND/1967032" xr:uid="{AA388262-B6EF-40CB-86F3-A8780C8CFE5C}"/>
+    <hyperlink ref="F9" r:id="rId3" display="https://www.digikey.com/products/en?keywords=350826-1" xr:uid="{AF2C5DAE-1F18-46E4-9165-DFED35C85B30}"/>
+    <hyperlink ref="F10" r:id="rId4" xr:uid="{C729E256-9F95-4A2D-B59F-0E1D96B031FF}"/>
+    <hyperlink ref="F16" r:id="rId5" xr:uid="{A1F256FE-A818-48FF-9A2B-6C63965D9F30}"/>
+    <hyperlink ref="F15" r:id="rId6" xr:uid="{0C93E5B3-066A-4EE0-A5C5-CD3026FD1BB5}"/>
+    <hyperlink ref="F17" r:id="rId7" xr:uid="{84FD6FA1-60F7-4C7F-B839-BB9816C4E1F5}"/>
+    <hyperlink ref="F32" r:id="rId8" xr:uid="{EF934DD1-1AA1-4E61-8CB1-0E6A5DD5C056}"/>
+    <hyperlink ref="F31" r:id="rId9" xr:uid="{059A2C48-0995-4C2C-9546-0AAFA69F18C7}"/>
+    <hyperlink ref="F30" r:id="rId10" xr:uid="{18472DCE-2DCD-4D8E-8715-A6B0EB7DCF6F}"/>
+    <hyperlink ref="F13" r:id="rId11" xr:uid="{6B63279A-20E1-4238-92A5-1F4C0BB4D2C6}"/>
+    <hyperlink ref="F14" r:id="rId12" display="https://www.digikey.com/products/en?keywords=B08B-PASK(LF)(SN)" xr:uid="{F7F63CA3-CC2F-4F26-BAC8-E722E15B0FE6}"/>
+    <hyperlink ref="F28" r:id="rId13" xr:uid="{7482BAB2-28E9-4ADA-AE57-C4F32D246C7D}"/>
+    <hyperlink ref="F29" r:id="rId14" xr:uid="{D6BCEDD3-6A5A-4736-ABC8-D4193B06B1EB}"/>
+    <hyperlink ref="F12" r:id="rId15" xr:uid="{9666A8FB-9135-479F-9241-64046C348EAA}"/>
+    <hyperlink ref="F24" r:id="rId16" display="https://www.digikey.com/product-detail/en/yageo/RC0805JR-070RL/311-0.0ARCT-ND/731163" xr:uid="{E5E3B2F9-A068-40F8-B6B9-C711BCCB8404}"/>
+    <hyperlink ref="F22" r:id="rId17" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0710KL/311-10.0KCRCT-ND/730482" xr:uid="{B7FA693C-E60B-4345-B18D-312724FF1AED}"/>
+    <hyperlink ref="F20" r:id="rId18" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-071KL/311-1.00KCRCT-ND/730391" xr:uid="{DBB35FAA-A217-4E29-A096-0A627004B5D8}"/>
+    <hyperlink ref="F21" r:id="rId19" xr:uid="{0556756C-052E-48D8-BAD1-B8296C581D77}"/>
+    <hyperlink ref="F23" r:id="rId20" xr:uid="{D79F8BDF-EA02-480A-B7D7-676926066110}"/>
+    <hyperlink ref="F25" r:id="rId21" xr:uid="{EB87A354-F8E8-4374-BD60-5AA576A83776}"/>
+    <hyperlink ref="F26" r:id="rId22" xr:uid="{5C7D045E-F0AE-4379-AB05-815D68D98529}"/>
+    <hyperlink ref="F27" r:id="rId23" xr:uid="{2433D550-04DB-4B89-A728-C8EB59B0A6A0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ref #6 Researched more components and added descriptions from the distrubuter. Addtionally, formatted the table.
</commit_message>
<xml_diff>
--- a/LegacyIOBoardBOM.xlsx
+++ b/LegacyIOBoardBOM.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aasleso\Documents\New-Hydra-Legacy-IO-Board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dedens\Documents\New-Hydra-Legacy-IO-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D38281-E81B-4D9A-A841-7D342EC4D6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D3196B-B8B6-4A50-9097-19316991CB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{E75E0199-A4FC-4142-9D32-2C5EB3346CD5}"/>
+    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{E75E0199-A4FC-4142-9D32-2C5EB3346CD5}"/>
   </bookViews>
   <sheets>
     <sheet name="LegacyIOBoard" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="123">
   <si>
     <t>Reference</t>
   </si>
@@ -244,9 +257,6 @@
     <t>311-1.00KCRCT-ND</t>
   </si>
   <si>
-    <t>Jumper resistors</t>
-  </si>
-  <si>
     <t>P56.2KHTR-ND</t>
   </si>
   <si>
@@ -263,13 +273,142 @@
   </si>
   <si>
     <t>CL21A106KOQNNNG</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>PL5 Brd Qty</t>
+  </si>
+  <si>
+    <t>Extended Cost</t>
+  </si>
+  <si>
+    <t>RJ45 Brd Qty</t>
+  </si>
+  <si>
+    <t>Jumper Resistors</t>
+  </si>
+  <si>
+    <t>RES SMD 0.0 OHM JUMPER 1/8W 0805</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>PL5 Board</t>
+  </si>
+  <si>
+    <t>RJ45 Board</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>RES 1K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 56.2K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>LED BLUE CLEAR 0805 SMD</t>
+  </si>
+  <si>
+    <t>DIODE STANDARD 100V 200MA SOT233</t>
+  </si>
+  <si>
+    <t>CONN HDR 4POS 0.25 TIN PCB</t>
+  </si>
+  <si>
+    <t>CONN MOD JACK 8P8C VERT SHIELDED</t>
+  </si>
+  <si>
+    <t>FO TRANSCEIVER, 4.25 GBPS, LC 850NM, SFF UNCOATED</t>
+  </si>
+  <si>
+    <t>CONN HDR 3POS 0.25 TIN PCB</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 8POS 2MM</t>
+  </si>
+  <si>
+    <t>Mod Debug</t>
+  </si>
+  <si>
+    <t>RELAY GEN PURPOSE SPDT 30A 12V</t>
+  </si>
+  <si>
+    <t>RELAY REED DPST 500MA 12V</t>
+  </si>
+  <si>
+    <t>RELAY GEN PURPOSE SPDT 10A 12V</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 9K OHM 0.5% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>RES SMD 49.9KOHM 0.1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RES 243 OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RES 16.2K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>IC REG BUCK ADJ 3A TSOT26</t>
+  </si>
+  <si>
+    <t>SBC 1.5GHZ 4 CORE 1GB RAM</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 30V 6.2A SOT23</t>
+  </si>
+  <si>
+    <t>OPTOISOLTR 5.3KV 1CH TRANS 4-SMD</t>
+  </si>
+  <si>
+    <t>IC REG BUCK ADJ 1.5A SOT23-6</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 16V X5R 0805</t>
+  </si>
+  <si>
+    <t>490-1313-2-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 16V X7R 0402</t>
+  </si>
+  <si>
+    <t>311-1088-2-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 16V X7R 0603</t>
+  </si>
+  <si>
+    <t>1276-3047-2-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 22UF 25V X5R 1206</t>
+  </si>
+  <si>
+    <t>CAP CER 100PF 50V C0G/NPO 0402</t>
+  </si>
+  <si>
+    <t>311-1024-2-ND</t>
+  </si>
+  <si>
+    <t>Daktronics Part Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,8 +551,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -595,12 +740,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="3" tint="0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -715,6 +878,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -761,32 +968,64 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="42" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="42" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1165,682 +1404,1275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6FEE036-4CF9-483C-8C65-E8C9586B780D}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="C3:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="49.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="86.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="49.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" customWidth="1"/>
+    <col min="12" max="12" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="D3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="I3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="K3" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="L3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C4" s="7">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="E4" s="7">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="G4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="8">
+        <f>L4*M4</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="6"/>
+      <c r="P4" s="8">
+        <f>L4*O4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C5" s="7">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2">
+      <c r="E5" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="G5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="8">
+        <f t="shared" ref="N5:N34" si="0">L5*M5</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="8">
+        <f t="shared" ref="P5:P34" si="1">L5*O5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C6" s="7">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2">
+      <c r="E6" s="7">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="G6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="K6" s="6"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="6"/>
+      <c r="P6" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C7" s="7">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2">
+      <c r="E7" s="7">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="G7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="6"/>
+      <c r="P7" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C8" s="7">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2">
+      <c r="E8" s="7">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="G8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K8" s="6"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="6"/>
+      <c r="P8" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C9" s="7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2">
+      <c r="E9" s="7">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="F9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="G9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="25" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="I9" s="9"/>
+      <c r="J9" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="6"/>
+      <c r="P9" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C10" s="7">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D10" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="2">
+      <c r="E10" s="7">
         <v>10</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="F10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="G10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="25" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="I10" s="9"/>
+      <c r="J10" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="6"/>
+      <c r="P10" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C11" s="7">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2">
+      <c r="E11" s="7">
         <v>1</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="F11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="G11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="25" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="I11" s="9"/>
+      <c r="J11" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" s="6"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="6"/>
+      <c r="P11" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C12" s="7">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="2">
+      <c r="E12" s="7">
         <v>8</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="F12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="G12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="25" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="I12" s="9"/>
+      <c r="J12" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="6"/>
+      <c r="P12" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C13" s="7">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="2">
+      <c r="E13" s="7">
         <v>8</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="F13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="G13" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H13" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="I13" s="6"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="6"/>
+      <c r="P13" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C14" s="7">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="2">
+      <c r="E14" s="7">
         <v>4</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="F14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="G14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="25" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="I14" s="9"/>
+      <c r="J14" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="6"/>
+      <c r="P14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C15" s="7">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="2">
+      <c r="E15" s="7">
         <v>8</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="F15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="4" t="s">
+      <c r="G15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="I15" s="9"/>
+      <c r="J15" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="6"/>
+      <c r="P15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C16" s="7">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="2">
+      <c r="E16" s="7">
         <v>1</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="F16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="G16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="25" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="I16" s="9"/>
+      <c r="J16" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="L16" s="8"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="6"/>
+      <c r="P16" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C17" s="7">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="2">
+      <c r="E17" s="7">
         <v>4</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="F17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="4" t="s">
+      <c r="G17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="25" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="I17" s="9"/>
+      <c r="J17" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="6"/>
+      <c r="P17" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C18" s="7">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="2">
+      <c r="E18" s="7">
         <v>4</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="F18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="4" t="s">
+      <c r="G18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="25" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="I18" s="9"/>
+      <c r="J18" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="K18" s="6"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="6"/>
+      <c r="P18" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C19" s="7">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="2">
+      <c r="E19" s="7">
         <v>2</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="F19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="4" t="s">
+      <c r="G19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="25" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="I19" s="9"/>
+      <c r="J19" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="K19" s="6"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="6"/>
+      <c r="P19" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C20" s="7">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="2">
+      <c r="E20" s="7">
         <v>1</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="F20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="G20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="6"/>
+      <c r="P20" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C21" s="7">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="2">
+      <c r="E21" s="7">
         <v>1</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="F21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="G21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="6"/>
+      <c r="P21" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C22" s="7">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="2">
+      <c r="E22" s="7">
         <v>12</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="F22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="4" t="s">
+      <c r="G22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" s="25" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="I22" s="9"/>
+      <c r="J22" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="K22" s="6"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="6"/>
+      <c r="P22" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C23" s="7">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
+      <c r="D23" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="2">
+      <c r="E23" s="7">
         <v>1</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="F23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" s="4" t="s">
+      <c r="G23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="K23" s="6"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="6"/>
+      <c r="P23" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C24" s="7">
+        <v>23</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="7">
+        <v>11</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="K24" s="6"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="6"/>
+      <c r="P24" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C25" s="7">
+        <v>24</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H25" s="25" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="I25" s="9"/>
+      <c r="J25" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K25" s="6"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="6"/>
+      <c r="P25" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="3:16" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C26" s="11">
+        <v>25</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="11">
+        <v>32</v>
+      </c>
+      <c r="F26" s="10">
+        <v>0</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" s="12"/>
+      <c r="J26" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="L26" s="13"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="14"/>
+      <c r="P26" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C27" s="7">
+        <v>26</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" s="9"/>
+      <c r="J27" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="K27" s="6"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="6"/>
+      <c r="P27" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C28" s="7">
+        <v>27</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="7">
+        <v>4</v>
+      </c>
+      <c r="F28" s="4">
+        <v>244</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="I28" s="9"/>
+      <c r="J28" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="K28" s="6"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O28" s="6"/>
+      <c r="P28" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C29" s="7">
+        <v>28</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="7">
+        <v>1</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="I29" s="9"/>
+      <c r="J29" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="K29" s="6"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="6"/>
+      <c r="P29" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C30" s="7">
+        <v>29</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="7">
+        <v>1</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="K30" s="6"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="6"/>
+      <c r="P30" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C31" s="7">
+        <v>30</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="7">
+        <v>1</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="I31" s="9"/>
+      <c r="J31" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K31" s="6"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="6"/>
+      <c r="P31" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C32" s="7">
         <v>31</v>
       </c>
-      <c r="C22" s="2">
-        <v>11</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="D32" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="7">
+        <v>10</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" s="9"/>
+      <c r="J32" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K32" s="6"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O32" s="6"/>
+      <c r="P32" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C33" s="7">
         <v>32</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>24</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="D33" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="7">
+        <v>4</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H33" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="I33" s="9"/>
+      <c r="J33" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="K33" s="6"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O33" s="6"/>
+      <c r="P33" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C34" s="7">
         <v>33</v>
       </c>
-      <c r="C23" s="2">
+      <c r="D34" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="7">
         <v>1</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="F34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H34" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" s="9"/>
+      <c r="J34" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="K34" s="6"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O34" s="6"/>
+      <c r="P34" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C35" s="7">
         <v>34</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>25</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="3">
-        <v>32</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="2">
+      <c r="D35" s="8"/>
+      <c r="E35" s="7">
         <v>1</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>27</v>
-      </c>
-      <c r="B26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="2">
-        <v>4</v>
-      </c>
-      <c r="D26" s="2">
-        <v>244</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>28</v>
-      </c>
-      <c r="B27" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="F35" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>31</v>
-      </c>
-      <c r="B30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="2">
-        <v>10</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="2">
-        <v>4</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>33</v>
-      </c>
-      <c r="B32" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>48</v>
+      <c r="G35" s="7"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="L35" s="8"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="8">
+        <f t="shared" ref="N35" si="2">L35*M35</f>
+        <v>0</v>
+      </c>
+      <c r="O35" s="6"/>
+      <c r="P35" s="8">
+        <f t="shared" ref="P35" si="3">L35*O35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="K36" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="16">
+        <f>SUM(N4:N35)</f>
+        <v>0</v>
+      </c>
+      <c r="O36" s="21"/>
+      <c r="P36" s="16">
+        <f>SUM(P4:P35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="K37" s="22"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="O37" s="23"/>
+      <c r="P37" s="17" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F7" r:id="rId1" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150080BS75000/732-4982-1-ND/4489910" xr:uid="{F28DB25A-81E7-42A4-91EF-90BD6F9ECF00}"/>
-    <hyperlink ref="F8" r:id="rId2" display="https://www.digikey.com/product-detail/en/on-semiconductor/BAS16LT3G/BAS16LT3GOSCT-ND/1967032" xr:uid="{AA388262-B6EF-40CB-86F3-A8780C8CFE5C}"/>
-    <hyperlink ref="F9" r:id="rId3" display="https://www.digikey.com/products/en?keywords=350826-1" xr:uid="{AF2C5DAE-1F18-46E4-9165-DFED35C85B30}"/>
-    <hyperlink ref="F10" r:id="rId4" xr:uid="{C729E256-9F95-4A2D-B59F-0E1D96B031FF}"/>
-    <hyperlink ref="F16" r:id="rId5" xr:uid="{A1F256FE-A818-48FF-9A2B-6C63965D9F30}"/>
-    <hyperlink ref="F15" r:id="rId6" xr:uid="{0C93E5B3-066A-4EE0-A5C5-CD3026FD1BB5}"/>
-    <hyperlink ref="F17" r:id="rId7" xr:uid="{84FD6FA1-60F7-4C7F-B839-BB9816C4E1F5}"/>
-    <hyperlink ref="F32" r:id="rId8" xr:uid="{EF934DD1-1AA1-4E61-8CB1-0E6A5DD5C056}"/>
-    <hyperlink ref="F31" r:id="rId9" xr:uid="{059A2C48-0995-4C2C-9546-0AAFA69F18C7}"/>
-    <hyperlink ref="F30" r:id="rId10" xr:uid="{18472DCE-2DCD-4D8E-8715-A6B0EB7DCF6F}"/>
-    <hyperlink ref="F13" r:id="rId11" xr:uid="{6B63279A-20E1-4238-92A5-1F4C0BB4D2C6}"/>
-    <hyperlink ref="F14" r:id="rId12" display="https://www.digikey.com/products/en?keywords=B08B-PASK(LF)(SN)" xr:uid="{F7F63CA3-CC2F-4F26-BAC8-E722E15B0FE6}"/>
-    <hyperlink ref="F28" r:id="rId13" xr:uid="{7482BAB2-28E9-4ADA-AE57-C4F32D246C7D}"/>
-    <hyperlink ref="F29" r:id="rId14" xr:uid="{D6BCEDD3-6A5A-4736-ABC8-D4193B06B1EB}"/>
-    <hyperlink ref="F12" r:id="rId15" xr:uid="{9666A8FB-9135-479F-9241-64046C348EAA}"/>
-    <hyperlink ref="F24" r:id="rId16" display="https://www.digikey.com/product-detail/en/yageo/RC0805JR-070RL/311-0.0ARCT-ND/731163" xr:uid="{E5E3B2F9-A068-40F8-B6B9-C711BCCB8404}"/>
-    <hyperlink ref="F22" r:id="rId17" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0710KL/311-10.0KCRCT-ND/730482" xr:uid="{B7FA693C-E60B-4345-B18D-312724FF1AED}"/>
-    <hyperlink ref="F20" r:id="rId18" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-071KL/311-1.00KCRCT-ND/730391" xr:uid="{DBB35FAA-A217-4E29-A096-0A627004B5D8}"/>
-    <hyperlink ref="F21" r:id="rId19" xr:uid="{0556756C-052E-48D8-BAD1-B8296C581D77}"/>
-    <hyperlink ref="F23" r:id="rId20" xr:uid="{D79F8BDF-EA02-480A-B7D7-676926066110}"/>
-    <hyperlink ref="F25" r:id="rId21" xr:uid="{EB87A354-F8E8-4374-BD60-5AA576A83776}"/>
-    <hyperlink ref="F26" r:id="rId22" xr:uid="{5C7D045E-F0AE-4379-AB05-815D68D98529}"/>
-    <hyperlink ref="F27" r:id="rId23" xr:uid="{2433D550-04DB-4B89-A728-C8EB59B0A6A0}"/>
+    <hyperlink ref="H9" r:id="rId1" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150080BS75000/732-4982-1-ND/4489910" xr:uid="{F28DB25A-81E7-42A4-91EF-90BD6F9ECF00}"/>
+    <hyperlink ref="H10" r:id="rId2" display="https://www.digikey.com/product-detail/en/on-semiconductor/BAS16LT3G/BAS16LT3GOSCT-ND/1967032" xr:uid="{AA388262-B6EF-40CB-86F3-A8780C8CFE5C}"/>
+    <hyperlink ref="H11" r:id="rId3" display="https://www.digikey.com/products/en?keywords=350826-1" xr:uid="{AF2C5DAE-1F18-46E4-9165-DFED35C85B30}"/>
+    <hyperlink ref="H12" r:id="rId4" xr:uid="{C729E256-9F95-4A2D-B59F-0E1D96B031FF}"/>
+    <hyperlink ref="H18" r:id="rId5" xr:uid="{A1F256FE-A818-48FF-9A2B-6C63965D9F30}"/>
+    <hyperlink ref="H17" r:id="rId6" xr:uid="{0C93E5B3-066A-4EE0-A5C5-CD3026FD1BB5}"/>
+    <hyperlink ref="H19" r:id="rId7" xr:uid="{84FD6FA1-60F7-4C7F-B839-BB9816C4E1F5}"/>
+    <hyperlink ref="H34" r:id="rId8" xr:uid="{EF934DD1-1AA1-4E61-8CB1-0E6A5DD5C056}"/>
+    <hyperlink ref="H33" r:id="rId9" xr:uid="{059A2C48-0995-4C2C-9546-0AAFA69F18C7}"/>
+    <hyperlink ref="H32" r:id="rId10" xr:uid="{18472DCE-2DCD-4D8E-8715-A6B0EB7DCF6F}"/>
+    <hyperlink ref="H15" r:id="rId11" xr:uid="{6B63279A-20E1-4238-92A5-1F4C0BB4D2C6}"/>
+    <hyperlink ref="H16" r:id="rId12" display="https://www.digikey.com/products/en?keywords=B08B-PASK(LF)(SN)" xr:uid="{F7F63CA3-CC2F-4F26-BAC8-E722E15B0FE6}"/>
+    <hyperlink ref="H30" r:id="rId13" xr:uid="{7482BAB2-28E9-4ADA-AE57-C4F32D246C7D}"/>
+    <hyperlink ref="H31" r:id="rId14" xr:uid="{D6BCEDD3-6A5A-4736-ABC8-D4193B06B1EB}"/>
+    <hyperlink ref="H14" r:id="rId15" xr:uid="{9666A8FB-9135-479F-9241-64046C348EAA}"/>
+    <hyperlink ref="H26" r:id="rId16" display="https://www.digikey.com/product-detail/en/yageo/RC0805JR-070RL/311-0.0ARCT-ND/731163" xr:uid="{E5E3B2F9-A068-40F8-B6B9-C711BCCB8404}"/>
+    <hyperlink ref="H24" r:id="rId17" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0710KL/311-10.0KCRCT-ND/730482" xr:uid="{B7FA693C-E60B-4345-B18D-312724FF1AED}"/>
+    <hyperlink ref="H22" r:id="rId18" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-071KL/311-1.00KCRCT-ND/730391" xr:uid="{DBB35FAA-A217-4E29-A096-0A627004B5D8}"/>
+    <hyperlink ref="H23" r:id="rId19" xr:uid="{0556756C-052E-48D8-BAD1-B8296C581D77}"/>
+    <hyperlink ref="H25" r:id="rId20" xr:uid="{D79F8BDF-EA02-480A-B7D7-676926066110}"/>
+    <hyperlink ref="H27" r:id="rId21" xr:uid="{EB87A354-F8E8-4374-BD60-5AA576A83776}"/>
+    <hyperlink ref="H28" r:id="rId22" xr:uid="{5C7D045E-F0AE-4379-AB05-815D68D98529}"/>
+    <hyperlink ref="H29" r:id="rId23" xr:uid="{2433D550-04DB-4B89-A728-C8EB59B0A6A0}"/>
+    <hyperlink ref="H4" r:id="rId24" xr:uid="{C0496564-6F2F-4051-A3E7-056A6272429B}"/>
+    <hyperlink ref="H5" r:id="rId25" xr:uid="{030AC6F1-D5A2-404E-9522-8A3DE0950CB3}"/>
+    <hyperlink ref="H7" r:id="rId26" xr:uid="{A66030A8-C9C0-4931-96AC-DE921E9622F4}"/>
+    <hyperlink ref="H8" r:id="rId27" xr:uid="{D28F7EA1-FE5F-4FF3-8C1A-1128EF7A0E4F}"/>
+    <hyperlink ref="H6" r:id="rId28" xr:uid="{55489D80-70BE-4344-A841-B910E217784F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ref #6 Added some Dak part numbers to the BOM.
</commit_message>
<xml_diff>
--- a/LegacyIOBoardBOM.xlsx
+++ b/LegacyIOBoardBOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dedens\Documents\New-Hydra-Legacy-IO-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D3196B-B8B6-4A50-9097-19316991CB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C942A4B2-9F09-4849-886F-D93B50B209D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{E75E0199-A4FC-4142-9D32-2C5EB3346CD5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="132">
   <si>
     <t>Reference</t>
   </si>
@@ -137,9 +137,6 @@
     <t>R4</t>
   </si>
   <si>
-    <t>9k</t>
-  </si>
-  <si>
     <t>R10,R26,R27,R28,R30,R31,R32,R38,R39,R40,R41,R42,R43,R44,R45,R46,R49,R50,R51,R52,R53,R54,R55,R56,R59,R60,R61,R62,R63,R64,R65,R66</t>
   </si>
   <si>
@@ -251,24 +248,6 @@
     <t>311-0.0ARCT-ND</t>
   </si>
   <si>
-    <t>311-10.0KCRCT-ND</t>
-  </si>
-  <si>
-    <t>311-1.00KCRCT-ND</t>
-  </si>
-  <si>
-    <t>P56.2KHTR-ND</t>
-  </si>
-  <si>
-    <t>13-RT1206DRE079KLTR-ND</t>
-  </si>
-  <si>
-    <t>P49.9KDCTR-ND</t>
-  </si>
-  <si>
-    <t>311-243LRTR-ND</t>
-  </si>
-  <si>
     <t>311-16.2KHRTR-ND</t>
   </si>
   <si>
@@ -305,12 +284,6 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>RES 1K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>RES SMD 56.2K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
     <t>LED BLUE CLEAR 0805 SMD</t>
   </si>
   <si>
@@ -344,18 +317,6 @@
     <t>RELAY GEN PURPOSE SPDT 10A 12V</t>
   </si>
   <si>
-    <t>RES 10K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>RES SMD 9K OHM 0.5% 1/4W 1206</t>
-  </si>
-  <si>
-    <t>RES SMD 49.9KOHM 0.1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>RES 243 OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
     <t>RES 16.2K OHM 1% 1/10W 0603</t>
   </si>
   <si>
@@ -402,6 +363,72 @@
   </si>
   <si>
     <t>Daktronics Part Number</t>
+  </si>
+  <si>
+    <t>P49.9KLTR-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 49.9K OHM 1% 1/10W 0402</t>
+  </si>
+  <si>
+    <t>R-1461</t>
+  </si>
+  <si>
+    <t>Voltage Divider</t>
+  </si>
+  <si>
+    <t>R-1339</t>
+  </si>
+  <si>
+    <t>311-243HRTR-ND</t>
+  </si>
+  <si>
+    <t>RES 243 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R-1465</t>
+  </si>
+  <si>
+    <t>R-1643</t>
+  </si>
+  <si>
+    <t>9.09k</t>
+  </si>
+  <si>
+    <t>R-1652</t>
+  </si>
+  <si>
+    <t>RES 9.09K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603FT9K09TR-ND</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>311-10KJRTR-ND</t>
+  </si>
+  <si>
+    <t>R-1424</t>
+  </si>
+  <si>
+    <t>R-1484</t>
+  </si>
+  <si>
+    <t>RES 56.2K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>YAG3187TR-ND</t>
+  </si>
+  <si>
+    <t>118-CR2010-JW-102ELFTR-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 5% 1/2W 2010</t>
+  </si>
+  <si>
+    <t>R-5051023</t>
   </si>
 </sst>
 </file>
@@ -1011,8 +1038,7 @@
     <xf numFmtId="0" fontId="16" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1028,6 +1054,7 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1407,7 +1434,7 @@
   <dimension ref="C3:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1419,7 +1446,7 @@
     <col min="5" max="5" width="9.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.109375" customWidth="1"/>
@@ -1432,7 +1459,7 @@
   <sheetData>
     <row r="3" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>0</v>
@@ -1444,34 +1471,34 @@
         <v>2</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.3">
@@ -1488,14 +1515,14 @@
         <v>4</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>79</v>
+        <v>68</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>72</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="8" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="8"/>
@@ -1524,14 +1551,14 @@
         <v>7</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>116</v>
+        <v>68</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>103</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="8" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="8"/>
@@ -1560,14 +1587,14 @@
         <v>9</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>121</v>
+        <v>68</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="8" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="8"/>
@@ -1596,14 +1623,14 @@
         <v>11</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>118</v>
+        <v>68</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>105</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="8" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="8"/>
@@ -1632,14 +1659,14 @@
         <v>13</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>114</v>
+        <v>68</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>101</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="8" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="8"/>
@@ -1668,14 +1695,14 @@
         <v>5</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>50</v>
+        <v>68</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="8" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="8"/>
@@ -1695,7 +1722,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="7">
         <v>10</v>
@@ -1704,14 +1731,14 @@
         <v>5</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H10" s="25" t="s">
-        <v>52</v>
+        <v>68</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>51</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="8" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="8"/>
@@ -1740,14 +1767,14 @@
         <v>5</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H11" s="25" t="s">
-        <v>55</v>
+        <v>68</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="8" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="8"/>
@@ -1767,7 +1794,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="7">
         <v>8</v>
@@ -1776,14 +1803,14 @@
         <v>5</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>58</v>
+        <v>68</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>57</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="8" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="8"/>
@@ -1811,14 +1838,16 @@
       <c r="F13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="24" t="s">
-        <v>70</v>
+      <c r="G13" s="23" t="s">
+        <v>69</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="19"/>
+        <v>58</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="18"/>
       <c r="K13" s="6"/>
       <c r="L13" s="8"/>
       <c r="M13" s="6"/>
@@ -1846,14 +1875,14 @@
         <v>5</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="I14" s="9"/>
-      <c r="J14" s="19" t="s">
-        <v>96</v>
+      <c r="J14" s="18" t="s">
+        <v>87</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="8"/>
@@ -1882,14 +1911,14 @@
         <v>5</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>64</v>
+        <v>68</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>63</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="15" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="8"/>
@@ -1918,17 +1947,17 @@
         <v>5</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="25" t="s">
-        <v>65</v>
+        <v>68</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>64</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="8" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="6"/>
@@ -1956,14 +1985,14 @@
         <v>5</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>61</v>
+        <v>68</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>60</v>
       </c>
       <c r="I17" s="9"/>
-      <c r="J17" s="18" t="s">
-        <v>100</v>
+      <c r="J17" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="K17" s="6"/>
       <c r="L17" s="8"/>
@@ -1992,14 +2021,14 @@
         <v>5</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>60</v>
+        <v>68</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>59</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="8" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="8"/>
@@ -2028,14 +2057,14 @@
         <v>5</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H19" s="25" t="s">
-        <v>62</v>
+        <v>68</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>61</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="8" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="8"/>
@@ -2064,7 +2093,7 @@
         <v>24</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="6"/>
@@ -2096,7 +2125,7 @@
         <v>26</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="6"/>
@@ -2128,14 +2157,16 @@
         <v>28</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H22" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="I22" s="9"/>
+        <v>68</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>131</v>
+      </c>
       <c r="J22" s="8" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="8"/>
@@ -2164,14 +2195,16 @@
         <v>30</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H23" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="I23" s="9"/>
+        <v>68</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="J23" s="8" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="K23" s="6"/>
       <c r="L23" s="8"/>
@@ -2200,14 +2233,16 @@
         <v>32</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H24" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="I24" s="9"/>
+        <v>68</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="J24" s="8" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="8"/>
@@ -2233,17 +2268,19 @@
         <v>1</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>34</v>
+        <v>119</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="I25" s="9"/>
+        <v>68</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>120</v>
+      </c>
       <c r="J25" s="8" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="K25" s="6"/>
       <c r="L25" s="8"/>
@@ -2262,8 +2299,8 @@
       <c r="C26" s="11">
         <v>25</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>35</v>
+      <c r="D26" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="E26" s="11">
         <v>32</v>
@@ -2272,17 +2309,19 @@
         <v>0</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H26" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="I26" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>114</v>
+      </c>
       <c r="J26" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="L26" s="13"/>
       <c r="M26" s="14"/>
@@ -2300,26 +2339,30 @@
       <c r="C27" s="7">
         <v>26</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>36</v>
+      <c r="D27" s="26" t="s">
+        <v>35</v>
       </c>
       <c r="E27" s="7">
         <v>1</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H27" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="I27" s="9"/>
+        <v>68</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>112</v>
+      </c>
       <c r="J27" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="K27" s="6"/>
+        <v>111</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="L27" s="8"/>
       <c r="M27" s="6"/>
       <c r="N27" s="8">
@@ -2337,23 +2380,25 @@
         <v>27</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E28" s="7">
         <v>4</v>
       </c>
       <c r="F28" s="4">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H28" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="I28" s="9"/>
+        <v>68</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>117</v>
+      </c>
       <c r="J28" s="8" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="K28" s="6"/>
       <c r="L28" s="8"/>
@@ -2373,23 +2418,25 @@
         <v>28</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E29" s="7">
         <v>1</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H29" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="I29" s="9"/>
+        <v>68</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>118</v>
+      </c>
       <c r="J29" s="8" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="K29" s="6"/>
       <c r="L29" s="8"/>
@@ -2409,7 +2456,7 @@
         <v>29</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E30" s="7">
         <v>1</v>
@@ -2418,14 +2465,14 @@
         <v>5</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H30" s="25" t="s">
-        <v>42</v>
+        <v>68</v>
+      </c>
+      <c r="H30" s="24" t="s">
+        <v>41</v>
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="8" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="K30" s="6"/>
       <c r="L30" s="8"/>
@@ -2445,7 +2492,7 @@
         <v>30</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31" s="7">
         <v>1</v>
@@ -2454,14 +2501,14 @@
         <v>5</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H31" s="25" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="H31" s="24" t="s">
+        <v>65</v>
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="8" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="K31" s="6"/>
       <c r="L31" s="8"/>
@@ -2481,7 +2528,7 @@
         <v>31</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E32" s="7">
         <v>10</v>
@@ -2490,14 +2537,14 @@
         <v>5</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H32" s="25" t="s">
-        <v>45</v>
+        <v>68</v>
+      </c>
+      <c r="H32" s="24" t="s">
+        <v>44</v>
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="8" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="K32" s="6"/>
       <c r="L32" s="8"/>
@@ -2517,7 +2564,7 @@
         <v>32</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E33" s="7">
         <v>4</v>
@@ -2526,14 +2573,14 @@
         <v>5</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H33" s="25" t="s">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c r="H33" s="24" t="s">
+        <v>62</v>
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="8" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="K33" s="6"/>
       <c r="L33" s="8"/>
@@ -2553,7 +2600,7 @@
         <v>33</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E34" s="7">
         <v>1</v>
@@ -2562,14 +2609,14 @@
         <v>5</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H34" s="25" t="s">
-        <v>48</v>
+        <v>68</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="8" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="K34" s="6"/>
       <c r="L34" s="8"/>
@@ -2596,11 +2643,11 @@
         <v>5</v>
       </c>
       <c r="G35" s="7"/>
-      <c r="H35" s="25"/>
+      <c r="H35" s="24"/>
       <c r="I35" s="9"/>
       <c r="J35" s="8"/>
       <c r="K35" s="6" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="L35" s="8"/>
       <c r="M35" s="6"/>
@@ -2616,30 +2663,30 @@
     </row>
     <row r="36" spans="3:16" x14ac:dyDescent="0.3">
       <c r="K36" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="L36" s="21"/>
-      <c r="M36" s="21"/>
+        <v>82</v>
+      </c>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
       <c r="N36" s="16">
         <f>SUM(N4:N35)</f>
         <v>0</v>
       </c>
-      <c r="O36" s="21"/>
+      <c r="O36" s="20"/>
       <c r="P36" s="16">
         <f>SUM(P4:P35)</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="K37" s="22"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="23"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
       <c r="N37" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="O37" s="23"/>
+        <v>80</v>
+      </c>
+      <c r="O37" s="22"/>
       <c r="P37" s="17" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2661,18 +2708,26 @@
     <hyperlink ref="H31" r:id="rId14" xr:uid="{D6BCEDD3-6A5A-4736-ABC8-D4193B06B1EB}"/>
     <hyperlink ref="H14" r:id="rId15" xr:uid="{9666A8FB-9135-479F-9241-64046C348EAA}"/>
     <hyperlink ref="H26" r:id="rId16" display="https://www.digikey.com/product-detail/en/yageo/RC0805JR-070RL/311-0.0ARCT-ND/731163" xr:uid="{E5E3B2F9-A068-40F8-B6B9-C711BCCB8404}"/>
-    <hyperlink ref="H24" r:id="rId17" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0710KL/311-10.0KCRCT-ND/730482" xr:uid="{B7FA693C-E60B-4345-B18D-312724FF1AED}"/>
-    <hyperlink ref="H22" r:id="rId18" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-071KL/311-1.00KCRCT-ND/730391" xr:uid="{DBB35FAA-A217-4E29-A096-0A627004B5D8}"/>
-    <hyperlink ref="H23" r:id="rId19" xr:uid="{0556756C-052E-48D8-BAD1-B8296C581D77}"/>
-    <hyperlink ref="H25" r:id="rId20" xr:uid="{D79F8BDF-EA02-480A-B7D7-676926066110}"/>
-    <hyperlink ref="H27" r:id="rId21" xr:uid="{EB87A354-F8E8-4374-BD60-5AA576A83776}"/>
-    <hyperlink ref="H28" r:id="rId22" xr:uid="{5C7D045E-F0AE-4379-AB05-815D68D98529}"/>
-    <hyperlink ref="H29" r:id="rId23" xr:uid="{2433D550-04DB-4B89-A728-C8EB59B0A6A0}"/>
-    <hyperlink ref="H4" r:id="rId24" xr:uid="{C0496564-6F2F-4051-A3E7-056A6272429B}"/>
-    <hyperlink ref="H5" r:id="rId25" xr:uid="{030AC6F1-D5A2-404E-9522-8A3DE0950CB3}"/>
-    <hyperlink ref="H7" r:id="rId26" xr:uid="{A66030A8-C9C0-4931-96AC-DE921E9622F4}"/>
-    <hyperlink ref="H8" r:id="rId27" xr:uid="{D28F7EA1-FE5F-4FF3-8C1A-1128EF7A0E4F}"/>
-    <hyperlink ref="H6" r:id="rId28" xr:uid="{55489D80-70BE-4344-A841-B910E217784F}"/>
+    <hyperlink ref="H29" r:id="rId17" xr:uid="{2433D550-04DB-4B89-A728-C8EB59B0A6A0}"/>
+    <hyperlink ref="H4" r:id="rId18" xr:uid="{C0496564-6F2F-4051-A3E7-056A6272429B}"/>
+    <hyperlink ref="H5" r:id="rId19" xr:uid="{030AC6F1-D5A2-404E-9522-8A3DE0950CB3}"/>
+    <hyperlink ref="H7" r:id="rId20" xr:uid="{A66030A8-C9C0-4931-96AC-DE921E9622F4}"/>
+    <hyperlink ref="H8" r:id="rId21" xr:uid="{D28F7EA1-FE5F-4FF3-8C1A-1128EF7A0E4F}"/>
+    <hyperlink ref="H6" r:id="rId22" xr:uid="{55489D80-70BE-4344-A841-B910E217784F}"/>
+    <hyperlink ref="H27" r:id="rId23" xr:uid="{CEED5B7F-8B70-49FE-BAEF-4F0F4CF311D5}"/>
+    <hyperlink ref="I27" r:id="rId24" xr:uid="{685CF014-65EA-4B3D-841B-2F30C22E9DB2}"/>
+    <hyperlink ref="I26" r:id="rId25" xr:uid="{FC8E4AA9-DD2F-4434-9365-2D1C54C5FE5B}"/>
+    <hyperlink ref="H28" r:id="rId26" xr:uid="{398D7822-9432-4D37-90FC-F6BED0D5A3B3}"/>
+    <hyperlink ref="I28" r:id="rId27" xr:uid="{46BE45A2-7289-43DF-ADF8-2A7CB4C5EF4F}"/>
+    <hyperlink ref="I29" r:id="rId28" xr:uid="{B9478E1E-41B7-47BE-90C0-AF5FCBCC1B1C}"/>
+    <hyperlink ref="I25" r:id="rId29" xr:uid="{AF7B9620-FA52-4D89-B0C0-0EC964CD4219}"/>
+    <hyperlink ref="H25" r:id="rId30" xr:uid="{82119B45-D93B-40E7-BBCA-D3E88836CDCE}"/>
+    <hyperlink ref="H24" r:id="rId31" xr:uid="{9CD802B6-4C3A-481D-B821-7ABDB4F68460}"/>
+    <hyperlink ref="I24" r:id="rId32" xr:uid="{1BC425DC-5DDC-474E-A7B8-2731643CA663}"/>
+    <hyperlink ref="I23" r:id="rId33" xr:uid="{DF10D946-8827-4A81-90A2-C24B3B80FDCE}"/>
+    <hyperlink ref="H23" r:id="rId34" xr:uid="{A0FEEC20-4372-4ECE-880A-FD94ED05336D}"/>
+    <hyperlink ref="H22" r:id="rId35" xr:uid="{C8572576-6A39-4AAD-B233-8A8D5DEB34B6}"/>
+    <hyperlink ref="I22" r:id="rId36" xr:uid="{964763A4-800F-4D8E-9570-3890B3B7C361}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ref #6 Added more Dak part numbers.
</commit_message>
<xml_diff>
--- a/LegacyIOBoardBOM.xlsx
+++ b/LegacyIOBoardBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dedens\Documents\New-Hydra-Legacy-IO-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C942A4B2-9F09-4849-886F-D93B50B209D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374D409A-1CD0-40D5-B3C4-58726FAB5158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{E75E0199-A4FC-4142-9D32-2C5EB3346CD5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="137">
   <si>
     <t>Reference</t>
   </si>
@@ -251,9 +251,6 @@
     <t>311-16.2KHRTR-ND</t>
   </si>
   <si>
-    <t>CL21A106KOQNNNG</t>
-  </si>
-  <si>
     <t>Unit Cost</t>
   </si>
   <si>
@@ -335,33 +332,9 @@
     <t>IC REG BUCK ADJ 1.5A SOT23-6</t>
   </si>
   <si>
-    <t>CAP CER 10UF 16V X5R 0805</t>
-  </si>
-  <si>
-    <t>490-1313-2-ND</t>
-  </si>
-  <si>
-    <t>CAP CER 10000PF 16V X7R 0402</t>
-  </si>
-  <si>
-    <t>311-1088-2-ND</t>
-  </si>
-  <si>
     <t>CAP CER 0.1UF 16V X7R 0603</t>
   </si>
   <si>
-    <t>1276-3047-2-ND</t>
-  </si>
-  <si>
-    <t>CAP CER 22UF 25V X5R 1206</t>
-  </si>
-  <si>
-    <t>CAP CER 100PF 50V C0G/NPO 0402</t>
-  </si>
-  <si>
-    <t>311-1024-2-ND</t>
-  </si>
-  <si>
     <t>Daktronics Part Number</t>
   </si>
   <si>
@@ -429,6 +402,48 @@
   </si>
   <si>
     <t>R-5051023</t>
+  </si>
+  <si>
+    <t>1276-1005-2-ND</t>
+  </si>
+  <si>
+    <t>C-1203</t>
+  </si>
+  <si>
+    <t>CAP CER 100PF 50V C0G/NP0 0402</t>
+  </si>
+  <si>
+    <t>490-5922-2-ND</t>
+  </si>
+  <si>
+    <t>C-3899490</t>
+  </si>
+  <si>
+    <t>CAP CER 22UF 25V X5R 0805</t>
+  </si>
+  <si>
+    <t>1276-CL21A226MAYNNNETR-ND</t>
+  </si>
+  <si>
+    <t>C-5310898</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 50V X7R 1210</t>
+  </si>
+  <si>
+    <t>1276-3387-2-ND</t>
+  </si>
+  <si>
+    <t>C-5619687</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 100V X7R 0603</t>
+  </si>
+  <si>
+    <t>490-4781-2-ND</t>
+  </si>
+  <si>
+    <t>C-3875286</t>
   </si>
 </sst>
 </file>
@@ -1054,7 +1069,9 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1434,7 +1451,7 @@
   <dimension ref="C3:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1446,7 +1463,7 @@
     <col min="5" max="5" width="9.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.109375" customWidth="1"/>
@@ -1477,7 +1494,7 @@
         <v>48</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>53</v>
@@ -1486,19 +1503,19 @@
         <v>55</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="P3" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.3">
@@ -1518,11 +1535,13 @@
         <v>68</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="I4" s="9"/>
+        <v>132</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>133</v>
+      </c>
       <c r="J4" s="8" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="8"/>
@@ -1554,11 +1573,13 @@
         <v>68</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="I5" s="9"/>
+        <v>123</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J5" s="8" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="8"/>
@@ -1590,11 +1611,13 @@
         <v>68</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="I6" s="9"/>
+        <v>126</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>127</v>
+      </c>
       <c r="J6" s="8" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="8"/>
@@ -1626,11 +1649,13 @@
         <v>68</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="I7" s="9"/>
+        <v>129</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>130</v>
+      </c>
       <c r="J7" s="8" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="8"/>
@@ -1662,11 +1687,13 @@
         <v>68</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="I8" s="9"/>
+        <v>135</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="J8" s="8" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="8"/>
@@ -1702,7 +1729,7 @@
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="8"/>
@@ -1738,7 +1765,7 @@
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="8"/>
@@ -1774,7 +1801,7 @@
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="8"/>
@@ -1810,7 +1837,7 @@
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="8"/>
@@ -1882,7 +1909,7 @@
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="8"/>
@@ -1918,7 +1945,7 @@
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="8"/>
@@ -1954,10 +1981,10 @@
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="K16" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="6"/>
@@ -1992,7 +2019,7 @@
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K17" s="6"/>
       <c r="L17" s="8"/>
@@ -2028,7 +2055,7 @@
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="8"/>
@@ -2064,7 +2091,7 @@
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="8"/>
@@ -2160,13 +2187,13 @@
         <v>68</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="8"/>
@@ -2198,13 +2225,13 @@
         <v>68</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="K23" s="6"/>
       <c r="L23" s="8"/>
@@ -2236,13 +2263,13 @@
         <v>68</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="8"/>
@@ -2268,19 +2295,19 @@
         <v>1</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>68</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="K25" s="6"/>
       <c r="L25" s="8"/>
@@ -2315,13 +2342,13 @@
         <v>70</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L26" s="13"/>
       <c r="M26" s="14"/>
@@ -2339,7 +2366,7 @@
       <c r="C27" s="7">
         <v>26</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E27" s="7">
@@ -2352,16 +2379,16 @@
         <v>68</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="L27" s="8"/>
       <c r="M27" s="6"/>
@@ -2392,13 +2419,13 @@
         <v>68</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="K28" s="6"/>
       <c r="L28" s="8"/>
@@ -2433,10 +2460,10 @@
         <v>71</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K29" s="6"/>
       <c r="L29" s="8"/>
@@ -2472,7 +2499,7 @@
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K30" s="6"/>
       <c r="L30" s="8"/>
@@ -2508,7 +2535,7 @@
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K31" s="6"/>
       <c r="L31" s="8"/>
@@ -2544,7 +2571,7 @@
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K32" s="6"/>
       <c r="L32" s="8"/>
@@ -2580,7 +2607,7 @@
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K33" s="6"/>
       <c r="L33" s="8"/>
@@ -2616,7 +2643,7 @@
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K34" s="6"/>
       <c r="L34" s="8"/>
@@ -2647,7 +2674,7 @@
       <c r="I35" s="9"/>
       <c r="J35" s="8"/>
       <c r="K35" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L35" s="8"/>
       <c r="M35" s="6"/>
@@ -2663,7 +2690,7 @@
     </row>
     <row r="36" spans="3:16" x14ac:dyDescent="0.3">
       <c r="K36" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L36" s="20"/>
       <c r="M36" s="20"/>
@@ -2682,11 +2709,11 @@
       <c r="L37" s="22"/>
       <c r="M37" s="22"/>
       <c r="N37" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O37" s="22"/>
       <c r="P37" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2709,25 +2736,30 @@
     <hyperlink ref="H14" r:id="rId15" xr:uid="{9666A8FB-9135-479F-9241-64046C348EAA}"/>
     <hyperlink ref="H26" r:id="rId16" display="https://www.digikey.com/product-detail/en/yageo/RC0805JR-070RL/311-0.0ARCT-ND/731163" xr:uid="{E5E3B2F9-A068-40F8-B6B9-C711BCCB8404}"/>
     <hyperlink ref="H29" r:id="rId17" xr:uid="{2433D550-04DB-4B89-A728-C8EB59B0A6A0}"/>
-    <hyperlink ref="H4" r:id="rId18" xr:uid="{C0496564-6F2F-4051-A3E7-056A6272429B}"/>
-    <hyperlink ref="H5" r:id="rId19" xr:uid="{030AC6F1-D5A2-404E-9522-8A3DE0950CB3}"/>
-    <hyperlink ref="H7" r:id="rId20" xr:uid="{A66030A8-C9C0-4931-96AC-DE921E9622F4}"/>
-    <hyperlink ref="H8" r:id="rId21" xr:uid="{D28F7EA1-FE5F-4FF3-8C1A-1128EF7A0E4F}"/>
-    <hyperlink ref="H6" r:id="rId22" xr:uid="{55489D80-70BE-4344-A841-B910E217784F}"/>
-    <hyperlink ref="H27" r:id="rId23" xr:uid="{CEED5B7F-8B70-49FE-BAEF-4F0F4CF311D5}"/>
-    <hyperlink ref="I27" r:id="rId24" xr:uid="{685CF014-65EA-4B3D-841B-2F30C22E9DB2}"/>
-    <hyperlink ref="I26" r:id="rId25" xr:uid="{FC8E4AA9-DD2F-4434-9365-2D1C54C5FE5B}"/>
-    <hyperlink ref="H28" r:id="rId26" xr:uid="{398D7822-9432-4D37-90FC-F6BED0D5A3B3}"/>
-    <hyperlink ref="I28" r:id="rId27" xr:uid="{46BE45A2-7289-43DF-ADF8-2A7CB4C5EF4F}"/>
-    <hyperlink ref="I29" r:id="rId28" xr:uid="{B9478E1E-41B7-47BE-90C0-AF5FCBCC1B1C}"/>
-    <hyperlink ref="I25" r:id="rId29" xr:uid="{AF7B9620-FA52-4D89-B0C0-0EC964CD4219}"/>
-    <hyperlink ref="H25" r:id="rId30" xr:uid="{82119B45-D93B-40E7-BBCA-D3E88836CDCE}"/>
-    <hyperlink ref="H24" r:id="rId31" xr:uid="{9CD802B6-4C3A-481D-B821-7ABDB4F68460}"/>
-    <hyperlink ref="I24" r:id="rId32" xr:uid="{1BC425DC-5DDC-474E-A7B8-2731643CA663}"/>
-    <hyperlink ref="I23" r:id="rId33" xr:uid="{DF10D946-8827-4A81-90A2-C24B3B80FDCE}"/>
-    <hyperlink ref="H23" r:id="rId34" xr:uid="{A0FEEC20-4372-4ECE-880A-FD94ED05336D}"/>
-    <hyperlink ref="H22" r:id="rId35" xr:uid="{C8572576-6A39-4AAD-B233-8A8D5DEB34B6}"/>
-    <hyperlink ref="I22" r:id="rId36" xr:uid="{964763A4-800F-4D8E-9570-3890B3B7C361}"/>
+    <hyperlink ref="H5" r:id="rId18" xr:uid="{030AC6F1-D5A2-404E-9522-8A3DE0950CB3}"/>
+    <hyperlink ref="H7" r:id="rId19" xr:uid="{A66030A8-C9C0-4931-96AC-DE921E9622F4}"/>
+    <hyperlink ref="H27" r:id="rId20" xr:uid="{CEED5B7F-8B70-49FE-BAEF-4F0F4CF311D5}"/>
+    <hyperlink ref="I27" r:id="rId21" xr:uid="{685CF014-65EA-4B3D-841B-2F30C22E9DB2}"/>
+    <hyperlink ref="I26" r:id="rId22" xr:uid="{FC8E4AA9-DD2F-4434-9365-2D1C54C5FE5B}"/>
+    <hyperlink ref="H28" r:id="rId23" xr:uid="{398D7822-9432-4D37-90FC-F6BED0D5A3B3}"/>
+    <hyperlink ref="I28" r:id="rId24" xr:uid="{46BE45A2-7289-43DF-ADF8-2A7CB4C5EF4F}"/>
+    <hyperlink ref="I29" r:id="rId25" xr:uid="{B9478E1E-41B7-47BE-90C0-AF5FCBCC1B1C}"/>
+    <hyperlink ref="I25" r:id="rId26" xr:uid="{AF7B9620-FA52-4D89-B0C0-0EC964CD4219}"/>
+    <hyperlink ref="H25" r:id="rId27" xr:uid="{82119B45-D93B-40E7-BBCA-D3E88836CDCE}"/>
+    <hyperlink ref="H24" r:id="rId28" xr:uid="{9CD802B6-4C3A-481D-B821-7ABDB4F68460}"/>
+    <hyperlink ref="I24" r:id="rId29" xr:uid="{1BC425DC-5DDC-474E-A7B8-2731643CA663}"/>
+    <hyperlink ref="I23" r:id="rId30" xr:uid="{DF10D946-8827-4A81-90A2-C24B3B80FDCE}"/>
+    <hyperlink ref="H23" r:id="rId31" xr:uid="{A0FEEC20-4372-4ECE-880A-FD94ED05336D}"/>
+    <hyperlink ref="H22" r:id="rId32" xr:uid="{C8572576-6A39-4AAD-B233-8A8D5DEB34B6}"/>
+    <hyperlink ref="I22" r:id="rId33" xr:uid="{964763A4-800F-4D8E-9570-3890B3B7C361}"/>
+    <hyperlink ref="I5" r:id="rId34" xr:uid="{5EAED019-2DC6-4DB6-9B1C-734614E01CCD}"/>
+    <hyperlink ref="H6" r:id="rId35" xr:uid="{7CF8FFD1-B58D-460F-AE89-2BFFE4128422}"/>
+    <hyperlink ref="I6" r:id="rId36" xr:uid="{F297F700-8069-4AA1-BF4D-684558C29C94}"/>
+    <hyperlink ref="I7" r:id="rId37" xr:uid="{87BA827C-5029-405E-AFBE-308F38B9CC2F}"/>
+    <hyperlink ref="H4" r:id="rId38" xr:uid="{87D0B601-D802-46BA-AD58-A2F419534684}"/>
+    <hyperlink ref="I4" r:id="rId39" xr:uid="{D34F74DE-4513-4675-86B7-B72010CDA423}"/>
+    <hyperlink ref="H8" r:id="rId40" xr:uid="{1BC87A8A-3B17-4BA1-9EDC-5B3E1E92AF9C}"/>
+    <hyperlink ref="I8" r:id="rId41" xr:uid="{79485DE8-CFF0-434A-A2ED-C2E532305F18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ref #6 Got prices almost finalized. Found more Daktronics part numbers. Highlighted sections that are still Work In Progress.
</commit_message>
<xml_diff>
--- a/LegacyIOBoardBOM.xlsx
+++ b/LegacyIOBoardBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dedens\Documents\New-Hydra-Legacy-IO-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC75A07F-A937-429A-9108-CE9AC09BCDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918E2D15-62E0-4B43-A8B1-B654192C1BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{E75E0199-A4FC-4142-9D32-2C5EB3346CD5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="147">
   <si>
     <t>Reference</t>
   </si>
@@ -371,9 +371,6 @@
     <t>R3,R5,R7,R8,R11,R13,R14,R18,R21,R24,R47,R57</t>
   </si>
   <si>
-    <t>33.2K</t>
-  </si>
-  <si>
     <t>U1,U2</t>
   </si>
   <si>
@@ -437,13 +434,58 @@
     <t>3.3uH</t>
   </si>
   <si>
-    <t>$</t>
-  </si>
-  <si>
     <t>JACK; 7 PIN, FEM, 1.27MM, SATA SLDR THRUHOLE</t>
   </si>
   <si>
-    <t>what is</t>
+    <t>SSW-120-01-T-D-LL-ND</t>
+  </si>
+  <si>
+    <t>Connector for Pi</t>
+  </si>
+  <si>
+    <t>CONN RCPT 40POS 0.1 TIN PCB</t>
+  </si>
+  <si>
+    <t>BAS16LT3GOSTR-ND</t>
+  </si>
+  <si>
+    <t>DIODE STANDARD 100V 200MA SOT233</t>
+  </si>
+  <si>
+    <t>587-3459-2-ND</t>
+  </si>
+  <si>
+    <t>L-5220007</t>
+  </si>
+  <si>
+    <t>RMCF0805JT33K0TR-ND</t>
+  </si>
+  <si>
+    <t>R-1361</t>
+  </si>
+  <si>
+    <t>RES 33K OHM 5% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>FIXED IND 3.3UH 3A 30 MOHM SMD</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">33.2K </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>33k</t>
+    </r>
+  </si>
+  <si>
+    <t>J-1323</t>
   </si>
 </sst>
 </file>
@@ -1058,7 +1100,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1088,9 +1129,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="37" borderId="10" xfId="42" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1467,10 +1509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6FEE036-4CF9-483C-8C65-E8C9586B780D}">
-  <dimension ref="C3:P32"/>
+  <dimension ref="C3:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1553,32 +1595,32 @@
       <c r="G4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="25" t="s">
         <v>100</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>98</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="L4" s="31">
+        <v>113</v>
+      </c>
+      <c r="L4" s="29">
         <v>0.27</v>
       </c>
       <c r="M4" s="6">
         <v>2</v>
       </c>
-      <c r="N4" s="31">
+      <c r="N4" s="29">
         <f>L4*M4</f>
         <v>0.54</v>
       </c>
       <c r="O4" s="6">
         <v>2</v>
       </c>
-      <c r="P4" s="31">
+      <c r="P4" s="29">
         <f>(L4*O4)</f>
         <v>0.54</v>
       </c>
@@ -1599,7 +1641,7 @@
       <c r="G5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="23" t="s">
         <v>90</v>
       </c>
       <c r="I5" s="9" t="s">
@@ -1609,23 +1651,23 @@
         <v>74</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="L5" s="31">
+        <v>114</v>
+      </c>
+      <c r="L5" s="29">
         <v>0.1</v>
       </c>
       <c r="M5" s="6">
         <v>2</v>
       </c>
-      <c r="N5" s="31">
-        <f t="shared" ref="N5:N30" si="0">L5*M5</f>
+      <c r="N5" s="29">
+        <f t="shared" ref="N5:N31" si="0">L5*M5</f>
         <v>0.2</v>
       </c>
       <c r="O5" s="6">
         <v>2</v>
       </c>
-      <c r="P5" s="31">
-        <f t="shared" ref="P5:P30" si="1">(L5*O5)</f>
+      <c r="P5" s="29">
+        <f t="shared" ref="P5:P31" si="1">(L5*O5)</f>
         <v>0.2</v>
       </c>
     </row>
@@ -1645,7 +1687,7 @@
       <c r="G6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="23" t="s">
         <v>93</v>
       </c>
       <c r="I6" s="9" t="s">
@@ -1655,22 +1697,22 @@
         <v>92</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L6" s="31">
+        <v>115</v>
+      </c>
+      <c r="L6" s="29">
         <v>0.1</v>
       </c>
       <c r="M6" s="6">
         <v>2</v>
       </c>
-      <c r="N6" s="31">
+      <c r="N6" s="29">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="O6" s="6">
         <v>2</v>
       </c>
-      <c r="P6" s="31">
+      <c r="P6" s="29">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
@@ -1691,7 +1733,7 @@
       <c r="G7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="23" t="s">
         <v>96</v>
       </c>
       <c r="I7" s="9" t="s">
@@ -1701,22 +1743,22 @@
         <v>95</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="L7" s="31">
+        <v>116</v>
+      </c>
+      <c r="L7" s="29">
         <v>0.11</v>
       </c>
       <c r="M7" s="6">
         <v>4</v>
       </c>
-      <c r="N7" s="31">
+      <c r="N7" s="29">
         <f t="shared" si="0"/>
         <v>0.44</v>
       </c>
       <c r="O7" s="6">
         <v>4</v>
       </c>
-      <c r="P7" s="31">
+      <c r="P7" s="29">
         <f t="shared" si="1"/>
         <v>0.44</v>
       </c>
@@ -1737,10 +1779,10 @@
       <c r="G8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="27" t="s">
         <v>4</v>
       </c>
       <c r="J8" s="8" t="s">
@@ -1749,20 +1791,20 @@
       <c r="K8" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="29">
         <v>0.19</v>
       </c>
       <c r="M8" s="6">
         <v>11</v>
       </c>
-      <c r="N8" s="31">
+      <c r="N8" s="29">
         <f t="shared" si="0"/>
         <v>2.09</v>
       </c>
       <c r="O8" s="6">
         <v>11</v>
       </c>
-      <c r="P8" s="31">
+      <c r="P8" s="29">
         <f t="shared" si="1"/>
         <v>2.09</v>
       </c>
@@ -1783,30 +1825,34 @@
       <c r="G9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="I9" s="29"/>
-      <c r="J9" s="8"/>
+      <c r="H9" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="K9" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="L9" s="31" t="s">
-        <v>134</v>
+      <c r="L9" s="29">
+        <v>0.1</v>
       </c>
       <c r="M9" s="6">
         <v>10</v>
       </c>
-      <c r="N9" s="31" t="e">
+      <c r="N9" s="29">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="O9" s="6">
         <v>10</v>
       </c>
-      <c r="P9" s="31" t="e">
+      <c r="P9" s="29">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.3">
@@ -1825,30 +1871,30 @@
       <c r="G10" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="29"/>
+      <c r="I10" s="28"/>
       <c r="J10" s="8" t="s">
         <v>61</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="L10" s="31">
+        <v>117</v>
+      </c>
+      <c r="L10" s="29">
         <v>1.28</v>
       </c>
       <c r="M10" s="6">
         <v>1</v>
       </c>
-      <c r="N10" s="31">
+      <c r="N10" s="29">
         <f t="shared" si="0"/>
         <v>1.28</v>
       </c>
       <c r="O10" s="6">
         <v>1</v>
       </c>
-      <c r="P10" s="31">
+      <c r="P10" s="29">
         <f t="shared" si="1"/>
         <v>1.28</v>
       </c>
@@ -1869,30 +1915,32 @@
       <c r="G11" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="29"/>
+      <c r="I11" s="27" t="s">
+        <v>4</v>
+      </c>
       <c r="J11" s="8" t="s">
         <v>62</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L11" s="31">
+        <v>118</v>
+      </c>
+      <c r="L11" s="29">
         <v>1.39</v>
       </c>
       <c r="M11" s="6">
         <v>0</v>
       </c>
-      <c r="N11" s="31">
+      <c r="N11" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O11" s="6">
         <v>8</v>
       </c>
-      <c r="P11" s="31">
+      <c r="P11" s="29">
         <f t="shared" si="1"/>
         <v>11.12</v>
       </c>
@@ -1910,7 +1958,7 @@
       <c r="F12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="22" t="s">
         <v>48</v>
       </c>
       <c r="H12" s="8" t="s">
@@ -1919,26 +1967,26 @@
       <c r="I12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="18" t="s">
-        <v>135</v>
+      <c r="J12" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L12" s="31">
+        <v>119</v>
+      </c>
+      <c r="L12" s="29">
         <v>0</v>
       </c>
       <c r="M12" s="6">
         <v>8</v>
       </c>
-      <c r="N12" s="31">
+      <c r="N12" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O12" s="6">
         <v>0</v>
       </c>
-      <c r="P12" s="31">
+      <c r="P12" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1956,35 +2004,35 @@
       <c r="F13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="32" t="s">
+      <c r="H13" s="30" t="s">
         <v>45</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J13" s="17" t="s">
         <v>63</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="L13" s="31">
+        <v>120</v>
+      </c>
+      <c r="L13" s="29">
         <v>0</v>
       </c>
       <c r="M13" s="6">
         <v>4</v>
       </c>
-      <c r="N13" s="31">
+      <c r="N13" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O13" s="6">
         <v>4</v>
       </c>
-      <c r="P13" s="31">
+      <c r="P13" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2005,30 +2053,30 @@
       <c r="G14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="29"/>
+      <c r="I14" s="28"/>
       <c r="J14" s="15" t="s">
         <v>64</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="L14" s="31">
+        <v>121</v>
+      </c>
+      <c r="L14" s="29">
         <v>0.54700000000000004</v>
       </c>
       <c r="M14" s="6">
         <v>8</v>
       </c>
-      <c r="N14" s="31">
+      <c r="N14" s="29">
         <f t="shared" si="0"/>
         <v>4.3760000000000003</v>
       </c>
       <c r="O14" s="6">
         <v>8</v>
       </c>
-      <c r="P14" s="31">
+      <c r="P14" s="29">
         <f t="shared" si="1"/>
         <v>4.3760000000000003</v>
       </c>
@@ -2049,30 +2097,32 @@
       <c r="G15" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="29"/>
+      <c r="I15" s="9" t="s">
+        <v>146</v>
+      </c>
       <c r="J15" s="8" t="s">
         <v>65</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L15" s="31">
+      <c r="L15" s="29">
         <v>0.39</v>
       </c>
       <c r="M15" s="6">
         <v>1</v>
       </c>
-      <c r="N15" s="31">
+      <c r="N15" s="29">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
       <c r="O15" s="6">
         <v>1</v>
       </c>
-      <c r="P15" s="31">
+      <c r="P15" s="29">
         <f t="shared" si="1"/>
         <v>0.39</v>
       </c>
@@ -2093,32 +2143,32 @@
       <c r="G16" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="27" t="s">
         <v>4</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>67</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="L16" s="31">
+        <v>122</v>
+      </c>
+      <c r="L16" s="29">
         <v>2.72</v>
       </c>
       <c r="M16" s="6">
         <v>4</v>
       </c>
-      <c r="N16" s="31">
+      <c r="N16" s="29">
         <f t="shared" si="0"/>
         <v>10.88</v>
       </c>
       <c r="O16" s="6">
         <v>4</v>
       </c>
-      <c r="P16" s="31">
+      <c r="P16" s="29">
         <f t="shared" si="1"/>
         <v>10.88</v>
       </c>
@@ -2139,32 +2189,32 @@
       <c r="G17" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="27" t="s">
         <v>4</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>68</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="L17" s="31">
+        <v>124</v>
+      </c>
+      <c r="L17" s="29">
         <v>3.21</v>
       </c>
       <c r="M17" s="6">
         <v>4</v>
       </c>
-      <c r="N17" s="31">
+      <c r="N17" s="29">
         <f t="shared" si="0"/>
         <v>12.84</v>
       </c>
       <c r="O17" s="6">
         <v>4</v>
       </c>
-      <c r="P17" s="31">
+      <c r="P17" s="29">
         <f t="shared" si="1"/>
         <v>12.84</v>
       </c>
@@ -2185,32 +2235,32 @@
       <c r="G18" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="H18" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="28" t="s">
+      <c r="I18" s="27" t="s">
         <v>4</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>69</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="L18" s="31">
+        <v>123</v>
+      </c>
+      <c r="L18" s="29">
         <v>1.41</v>
       </c>
       <c r="M18" s="6">
         <v>2</v>
       </c>
-      <c r="N18" s="31">
+      <c r="N18" s="29">
         <f t="shared" si="0"/>
         <v>2.82</v>
       </c>
       <c r="O18" s="6">
         <v>2</v>
       </c>
-      <c r="P18" s="31">
+      <c r="P18" s="29">
         <f t="shared" si="1"/>
         <v>2.82</v>
       </c>
@@ -2226,33 +2276,39 @@
         <v>1</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="8"/>
+      <c r="H19" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="K19" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="L19" s="31" t="s">
-        <v>134</v>
+        <v>125</v>
+      </c>
+      <c r="L19" s="29">
+        <v>0.23</v>
       </c>
       <c r="M19" s="6">
         <v>1</v>
       </c>
-      <c r="N19" s="31" t="e">
+      <c r="N19" s="29">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>0.23</v>
       </c>
       <c r="O19" s="6">
         <v>1</v>
       </c>
-      <c r="P19" s="31" t="e">
+      <c r="P19" s="29">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.3">
@@ -2271,7 +2327,7 @@
       <c r="G20" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="H20" s="23" t="s">
         <v>87</v>
       </c>
       <c r="I20" s="9" t="s">
@@ -2281,22 +2337,22 @@
         <v>88</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="L20" s="31">
+        <v>126</v>
+      </c>
+      <c r="L20" s="29">
         <v>0.17</v>
       </c>
       <c r="M20" s="6">
         <v>11</v>
       </c>
-      <c r="N20" s="31">
+      <c r="N20" s="29">
         <f t="shared" si="0"/>
         <v>1.87</v>
       </c>
       <c r="O20" s="6">
         <v>11</v>
       </c>
-      <c r="P20" s="31">
+      <c r="P20" s="29">
         <f t="shared" si="1"/>
         <v>1.87</v>
       </c>
@@ -2317,7 +2373,7 @@
       <c r="G21" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="24" t="s">
+      <c r="H21" s="23" t="s">
         <v>86</v>
       </c>
       <c r="I21" s="9" t="s">
@@ -2329,20 +2385,20 @@
       <c r="K21" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="L21" s="31">
+      <c r="L21" s="29">
         <v>0.1</v>
       </c>
       <c r="M21" s="6">
         <v>1</v>
       </c>
-      <c r="N21" s="31">
+      <c r="N21" s="29">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="O21" s="6">
         <v>1</v>
       </c>
-      <c r="P21" s="31">
+      <c r="P21" s="29">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
@@ -2363,7 +2419,7 @@
       <c r="G22" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="24" t="s">
+      <c r="H22" s="23" t="s">
         <v>82</v>
       </c>
       <c r="I22" s="9" t="s">
@@ -2372,23 +2428,23 @@
       <c r="J22" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="K22" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="L22" s="31">
+      <c r="K22" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="L22" s="29">
         <v>0.1</v>
       </c>
       <c r="M22" s="6">
         <v>12</v>
       </c>
-      <c r="N22" s="31">
+      <c r="N22" s="29">
         <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="O22" s="6">
         <v>12</v>
       </c>
-      <c r="P22" s="31">
+      <c r="P22" s="29">
         <f t="shared" si="1"/>
         <v>1.2000000000000002</v>
       </c>
@@ -2404,40 +2460,46 @@
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H23" s="24"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="8"/>
+      <c r="H23" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="K23" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="L23" s="31" t="s">
-        <v>134</v>
+      <c r="L23" s="29">
+        <v>0.1</v>
       </c>
       <c r="M23" s="6">
         <v>1</v>
       </c>
-      <c r="N23" s="31" t="e">
+      <c r="N23" s="29">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>0.1</v>
       </c>
       <c r="O23" s="6">
         <v>1</v>
       </c>
-      <c r="P23" s="31" t="e">
+      <c r="P23" s="29">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="24" spans="3:16" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C24" s="11">
         <v>25</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="18" t="s">
         <v>22</v>
       </c>
       <c r="E24" s="11">
@@ -2449,7 +2511,7 @@
       <c r="G24" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="25" t="s">
+      <c r="H24" s="24" t="s">
         <v>49</v>
       </c>
       <c r="I24" s="12" t="s">
@@ -2461,20 +2523,20 @@
       <c r="K24" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="31">
+      <c r="L24" s="29">
         <v>0.1</v>
       </c>
       <c r="M24" s="14">
         <v>16</v>
       </c>
-      <c r="N24" s="31">
+      <c r="N24" s="29">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
       <c r="O24" s="14">
         <v>16</v>
       </c>
-      <c r="P24" s="31">
+      <c r="P24" s="29">
         <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
@@ -2495,7 +2557,7 @@
       <c r="G25" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H25" s="24" t="s">
+      <c r="H25" s="23" t="s">
         <v>78</v>
       </c>
       <c r="I25" s="9" t="s">
@@ -2505,22 +2567,22 @@
         <v>79</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="L25" s="31">
+        <v>128</v>
+      </c>
+      <c r="L25" s="29">
         <v>0.1</v>
       </c>
       <c r="M25" s="6">
         <v>4</v>
       </c>
-      <c r="N25" s="31">
+      <c r="N25" s="29">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="O25" s="6">
         <v>4</v>
       </c>
-      <c r="P25" s="31">
+      <c r="P25" s="29">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
@@ -2530,7 +2592,7 @@
         <v>29</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E26" s="7">
         <v>2</v>
@@ -2541,32 +2603,32 @@
       <c r="G26" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H26" s="24" t="s">
+      <c r="H26" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="28" t="s">
+      <c r="I26" s="27" t="s">
         <v>4</v>
       </c>
       <c r="J26" s="8" t="s">
         <v>70</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="L26" s="31">
+        <v>129</v>
+      </c>
+      <c r="L26" s="29">
         <v>0.3</v>
       </c>
       <c r="M26" s="6">
         <v>2</v>
       </c>
-      <c r="N26" s="31">
+      <c r="N26" s="29">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="O26" s="6">
         <v>2</v>
       </c>
-      <c r="P26" s="31">
+      <c r="P26" s="29">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
@@ -2587,45 +2649,43 @@
       <c r="G27" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="24" t="s">
+      <c r="H27" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="I27" s="28" t="s">
+      <c r="I27" s="27" t="s">
         <v>4</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>71</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="L27" s="31">
+        <v>130</v>
+      </c>
+      <c r="L27" s="29">
         <v>35</v>
       </c>
       <c r="M27" s="6">
         <v>1</v>
       </c>
-      <c r="N27" s="31">
+      <c r="N27" s="29">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="O27" s="6">
         <v>1</v>
       </c>
-      <c r="P27" s="31">
+      <c r="P27" s="29">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C28" s="7">
-        <v>31</v>
-      </c>
+      <c r="C28" s="7"/>
       <c r="D28" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E28" s="7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>4</v>
@@ -2633,143 +2693,189 @@
       <c r="G28" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H28" s="24" t="s">
+      <c r="H28" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="I28" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="L28" s="29">
+        <v>3.98</v>
+      </c>
+      <c r="M28" s="6">
+        <v>1</v>
+      </c>
+      <c r="N28" s="29">
+        <f t="shared" si="0"/>
+        <v>3.98</v>
+      </c>
+      <c r="O28" s="6">
+        <v>1</v>
+      </c>
+      <c r="P28" s="29">
+        <f t="shared" si="1"/>
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C29" s="7">
+        <v>31</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="7">
+        <v>10</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="I28" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="J28" s="8" t="s">
+      <c r="I29" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="K28" s="6" t="s">
+      <c r="K29" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L28" s="31">
+      <c r="L29" s="29">
         <v>0.48</v>
       </c>
-      <c r="M28" s="6">
+      <c r="M29" s="6">
         <v>10</v>
       </c>
-      <c r="N28" s="31">
+      <c r="N29" s="29">
         <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
-      <c r="O28" s="6">
+      <c r="O29" s="6">
         <v>10</v>
       </c>
-      <c r="P28" s="31">
+      <c r="P29" s="29">
         <f t="shared" si="1"/>
         <v>4.8</v>
       </c>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C29" s="7">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C30" s="7">
         <v>32</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="7">
-        <v>4</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" s="7" t="s">
+      <c r="E30" s="7">
+        <v>4</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H29" s="24" t="s">
+      <c r="H30" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="I29" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="8" t="s">
+      <c r="I30" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="K29" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="L29" s="31">
+      <c r="K30" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="L30" s="29">
         <v>0.87</v>
       </c>
-      <c r="M29" s="6">
-        <v>4</v>
-      </c>
-      <c r="N29" s="31">
+      <c r="M30" s="6">
+        <v>4</v>
+      </c>
+      <c r="N30" s="29">
         <f t="shared" si="0"/>
         <v>3.48</v>
       </c>
-      <c r="O29" s="6">
-        <v>4</v>
-      </c>
-      <c r="P29" s="31">
+      <c r="O30" s="6">
+        <v>4</v>
+      </c>
+      <c r="P30" s="29">
         <f t="shared" si="1"/>
         <v>3.48</v>
       </c>
     </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C30" s="7">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C31" s="7">
         <v>34</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="7">
+      <c r="D31" s="8"/>
+      <c r="E31" s="7">
         <v>1</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G30" s="7"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="6" t="s">
+      <c r="F31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="L30" s="31">
+      <c r="L31" s="29">
         <v>0</v>
       </c>
-      <c r="M30" s="6">
+      <c r="M31" s="6">
         <v>1</v>
       </c>
-      <c r="N30" s="31">
+      <c r="N31" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O30" s="6">
+      <c r="O31" s="6">
         <v>1</v>
       </c>
-      <c r="P30" s="31">
+      <c r="P31" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="K31" s="17" t="s">
+    <row r="32" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="K32" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="16" t="e">
-        <f>SUM(N4:N30)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O31" s="20"/>
-      <c r="P31" s="16" t="e">
-        <f>SUM(P4:P30)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="32" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="K32" s="21"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="17" t="s">
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="32">
+        <f>SUM(N4:N31)</f>
+        <v>90.416000000000011</v>
+      </c>
+      <c r="O32" s="19"/>
+      <c r="P32" s="32">
+        <f>SUM(P4:P31)</f>
+        <v>101.536</v>
+      </c>
+    </row>
+    <row r="33" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="K33" s="20"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="O32" s="22"/>
-      <c r="P32" s="17" t="s">
+      <c r="O33" s="21"/>
+      <c r="P33" s="16" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2782,8 +2888,8 @@
     <hyperlink ref="H17" r:id="rId4" xr:uid="{A1F256FE-A818-48FF-9A2B-6C63965D9F30}"/>
     <hyperlink ref="H16" r:id="rId5" xr:uid="{0C93E5B3-066A-4EE0-A5C5-CD3026FD1BB5}"/>
     <hyperlink ref="H18" r:id="rId6" xr:uid="{84FD6FA1-60F7-4C7F-B839-BB9816C4E1F5}"/>
-    <hyperlink ref="H29" r:id="rId7" xr:uid="{059A2C48-0995-4C2C-9546-0AAFA69F18C7}"/>
-    <hyperlink ref="H28" r:id="rId8" xr:uid="{18472DCE-2DCD-4D8E-8715-A6B0EB7DCF6F}"/>
+    <hyperlink ref="H30" r:id="rId7" xr:uid="{059A2C48-0995-4C2C-9546-0AAFA69F18C7}"/>
+    <hyperlink ref="H29" r:id="rId8" xr:uid="{18472DCE-2DCD-4D8E-8715-A6B0EB7DCF6F}"/>
     <hyperlink ref="H14" r:id="rId9" xr:uid="{6B63279A-20E1-4238-92A5-1F4C0BB4D2C6}"/>
     <hyperlink ref="H15" r:id="rId10" display="https://www.digikey.com/products/en?keywords=B08B-PASK(LF)(SN)" xr:uid="{F7F63CA3-CC2F-4F26-BAC8-E722E15B0FE6}"/>
     <hyperlink ref="H26" r:id="rId11" xr:uid="{7482BAB2-28E9-4ADA-AE57-C4F32D246C7D}"/>
@@ -2807,6 +2913,13 @@
     <hyperlink ref="H4" r:id="rId29" xr:uid="{87D0B601-D802-46BA-AD58-A2F419534684}"/>
     <hyperlink ref="I4" r:id="rId30" xr:uid="{D34F74DE-4513-4675-86B7-B72010CDA423}"/>
     <hyperlink ref="I12" r:id="rId31" xr:uid="{AA1B7A61-016A-4386-A80E-C48A0F92B9C3}"/>
+    <hyperlink ref="H28" r:id="rId32" xr:uid="{309E8561-9A75-49EF-9F97-555DAB8708F5}"/>
+    <hyperlink ref="H9" r:id="rId33" xr:uid="{9B214B05-19D6-4809-BB90-5084C9282352}"/>
+    <hyperlink ref="H19" r:id="rId34" xr:uid="{033F72ED-1B29-46A9-A448-EBCFB95409D6}"/>
+    <hyperlink ref="I19" r:id="rId35" xr:uid="{9AE40410-5209-463C-A59A-BDFA92BB1488}"/>
+    <hyperlink ref="H23" r:id="rId36" xr:uid="{D07650AF-6B66-4409-B8B3-C7A699BCD2BE}"/>
+    <hyperlink ref="I23" r:id="rId37" xr:uid="{004937F0-BC3D-4F72-B64D-3D6CBBEF8D0D}"/>
+    <hyperlink ref="I15" r:id="rId38" xr:uid="{2AB22E42-DD5F-447B-968A-2EAB2A752C71}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ref #6 Could not find the Dak part numbers for a few of the components.
</commit_message>
<xml_diff>
--- a/LegacyIOBoardBOM.xlsx
+++ b/LegacyIOBoardBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dedens\Documents\New-Hydra-Legacy-IO-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918E2D15-62E0-4B43-A8B1-B654192C1BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AFD297-4F30-4B92-B13A-FAAA77704A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{E75E0199-A4FC-4142-9D32-2C5EB3346CD5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="147">
   <si>
     <t>Reference</t>
   </si>
@@ -645,7 +645,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -846,12 +846,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1061,7 +1055,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1128,7 +1122,6 @@
     <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="10" xfId="42" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1512,7 +1505,7 @@
   <dimension ref="C3:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1607,20 +1600,20 @@
       <c r="K4" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="L4" s="29">
+      <c r="L4" s="28">
         <v>0.27</v>
       </c>
       <c r="M4" s="6">
         <v>2</v>
       </c>
-      <c r="N4" s="29">
+      <c r="N4" s="28">
         <f>L4*M4</f>
         <v>0.54</v>
       </c>
       <c r="O4" s="6">
         <v>2</v>
       </c>
-      <c r="P4" s="29">
+      <c r="P4" s="28">
         <f>(L4*O4)</f>
         <v>0.54</v>
       </c>
@@ -1653,20 +1646,20 @@
       <c r="K5" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="L5" s="29">
+      <c r="L5" s="28">
         <v>0.1</v>
       </c>
       <c r="M5" s="6">
         <v>2</v>
       </c>
-      <c r="N5" s="29">
+      <c r="N5" s="28">
         <f t="shared" ref="N5:N31" si="0">L5*M5</f>
         <v>0.2</v>
       </c>
       <c r="O5" s="6">
         <v>2</v>
       </c>
-      <c r="P5" s="29">
+      <c r="P5" s="28">
         <f t="shared" ref="P5:P31" si="1">(L5*O5)</f>
         <v>0.2</v>
       </c>
@@ -1699,20 +1692,20 @@
       <c r="K6" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="L6" s="29">
+      <c r="L6" s="28">
         <v>0.1</v>
       </c>
       <c r="M6" s="6">
         <v>2</v>
       </c>
-      <c r="N6" s="29">
+      <c r="N6" s="28">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="O6" s="6">
         <v>2</v>
       </c>
-      <c r="P6" s="29">
+      <c r="P6" s="28">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
@@ -1745,20 +1738,20 @@
       <c r="K7" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="L7" s="29">
+      <c r="L7" s="28">
         <v>0.11</v>
       </c>
       <c r="M7" s="6">
         <v>4</v>
       </c>
-      <c r="N7" s="29">
+      <c r="N7" s="28">
         <f t="shared" si="0"/>
         <v>0.44</v>
       </c>
       <c r="O7" s="6">
         <v>4</v>
       </c>
-      <c r="P7" s="29">
+      <c r="P7" s="28">
         <f t="shared" si="1"/>
         <v>0.44</v>
       </c>
@@ -1791,20 +1784,20 @@
       <c r="K8" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="29">
+      <c r="L8" s="28">
         <v>0.19</v>
       </c>
       <c r="M8" s="6">
         <v>11</v>
       </c>
-      <c r="N8" s="29">
+      <c r="N8" s="28">
         <f t="shared" si="0"/>
         <v>2.09</v>
       </c>
       <c r="O8" s="6">
         <v>11</v>
       </c>
-      <c r="P8" s="29">
+      <c r="P8" s="28">
         <f t="shared" si="1"/>
         <v>2.09</v>
       </c>
@@ -1837,20 +1830,20 @@
       <c r="K9" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="L9" s="29">
+      <c r="L9" s="28">
         <v>0.1</v>
       </c>
       <c r="M9" s="6">
         <v>10</v>
       </c>
-      <c r="N9" s="29">
+      <c r="N9" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O9" s="6">
         <v>10</v>
       </c>
-      <c r="P9" s="29">
+      <c r="P9" s="28">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1874,27 +1867,29 @@
       <c r="H10" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="28"/>
+      <c r="I10" s="27" t="s">
+        <v>4</v>
+      </c>
       <c r="J10" s="8" t="s">
         <v>61</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="28">
         <v>1.28</v>
       </c>
       <c r="M10" s="6">
         <v>1</v>
       </c>
-      <c r="N10" s="29">
+      <c r="N10" s="28">
         <f t="shared" si="0"/>
         <v>1.28</v>
       </c>
       <c r="O10" s="6">
         <v>1</v>
       </c>
-      <c r="P10" s="29">
+      <c r="P10" s="28">
         <f t="shared" si="1"/>
         <v>1.28</v>
       </c>
@@ -1927,20 +1922,20 @@
       <c r="K11" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L11" s="28">
         <v>1.39</v>
       </c>
       <c r="M11" s="6">
         <v>0</v>
       </c>
-      <c r="N11" s="29">
+      <c r="N11" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O11" s="6">
         <v>8</v>
       </c>
-      <c r="P11" s="29">
+      <c r="P11" s="28">
         <f t="shared" si="1"/>
         <v>11.12</v>
       </c>
@@ -1973,20 +1968,20 @@
       <c r="K12" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L12" s="29">
+      <c r="L12" s="28">
         <v>0</v>
       </c>
       <c r="M12" s="6">
         <v>8</v>
       </c>
-      <c r="N12" s="29">
+      <c r="N12" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O12" s="6">
         <v>0</v>
       </c>
-      <c r="P12" s="29">
+      <c r="P12" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2007,7 +2002,7 @@
       <c r="G13" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="29" t="s">
         <v>45</v>
       </c>
       <c r="I13" s="9" t="s">
@@ -2019,20 +2014,20 @@
       <c r="K13" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="L13" s="29">
+      <c r="L13" s="28">
         <v>0</v>
       </c>
       <c r="M13" s="6">
         <v>4</v>
       </c>
-      <c r="N13" s="29">
+      <c r="N13" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O13" s="6">
         <v>4</v>
       </c>
-      <c r="P13" s="29">
+      <c r="P13" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2056,27 +2051,29 @@
       <c r="H14" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="28"/>
+      <c r="I14" s="27" t="s">
+        <v>4</v>
+      </c>
       <c r="J14" s="15" t="s">
         <v>64</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="L14" s="29">
+      <c r="L14" s="28">
         <v>0.54700000000000004</v>
       </c>
       <c r="M14" s="6">
         <v>8</v>
       </c>
-      <c r="N14" s="29">
+      <c r="N14" s="28">
         <f t="shared" si="0"/>
         <v>4.3760000000000003</v>
       </c>
       <c r="O14" s="6">
         <v>8</v>
       </c>
-      <c r="P14" s="29">
+      <c r="P14" s="28">
         <f t="shared" si="1"/>
         <v>4.3760000000000003</v>
       </c>
@@ -2109,20 +2106,20 @@
       <c r="K15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L15" s="29">
+      <c r="L15" s="28">
         <v>0.39</v>
       </c>
       <c r="M15" s="6">
         <v>1</v>
       </c>
-      <c r="N15" s="29">
+      <c r="N15" s="28">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
       <c r="O15" s="6">
         <v>1</v>
       </c>
-      <c r="P15" s="29">
+      <c r="P15" s="28">
         <f t="shared" si="1"/>
         <v>0.39</v>
       </c>
@@ -2155,20 +2152,20 @@
       <c r="K16" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="L16" s="29">
+      <c r="L16" s="28">
         <v>2.72</v>
       </c>
       <c r="M16" s="6">
         <v>4</v>
       </c>
-      <c r="N16" s="29">
+      <c r="N16" s="28">
         <f t="shared" si="0"/>
         <v>10.88</v>
       </c>
       <c r="O16" s="6">
         <v>4</v>
       </c>
-      <c r="P16" s="29">
+      <c r="P16" s="28">
         <f t="shared" si="1"/>
         <v>10.88</v>
       </c>
@@ -2201,20 +2198,20 @@
       <c r="K17" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="L17" s="29">
+      <c r="L17" s="28">
         <v>3.21</v>
       </c>
       <c r="M17" s="6">
         <v>4</v>
       </c>
-      <c r="N17" s="29">
+      <c r="N17" s="28">
         <f t="shared" si="0"/>
         <v>12.84</v>
       </c>
       <c r="O17" s="6">
         <v>4</v>
       </c>
-      <c r="P17" s="29">
+      <c r="P17" s="28">
         <f t="shared" si="1"/>
         <v>12.84</v>
       </c>
@@ -2247,20 +2244,20 @@
       <c r="K18" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="L18" s="29">
+      <c r="L18" s="28">
         <v>1.41</v>
       </c>
       <c r="M18" s="6">
         <v>2</v>
       </c>
-      <c r="N18" s="29">
+      <c r="N18" s="28">
         <f t="shared" si="0"/>
         <v>2.82</v>
       </c>
       <c r="O18" s="6">
         <v>2</v>
       </c>
-      <c r="P18" s="29">
+      <c r="P18" s="28">
         <f t="shared" si="1"/>
         <v>2.82</v>
       </c>
@@ -2293,20 +2290,20 @@
       <c r="K19" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="L19" s="29">
+      <c r="L19" s="28">
         <v>0.23</v>
       </c>
       <c r="M19" s="6">
         <v>1</v>
       </c>
-      <c r="N19" s="29">
+      <c r="N19" s="28">
         <f t="shared" si="0"/>
         <v>0.23</v>
       </c>
       <c r="O19" s="6">
         <v>1</v>
       </c>
-      <c r="P19" s="29">
+      <c r="P19" s="28">
         <f t="shared" si="1"/>
         <v>0.23</v>
       </c>
@@ -2339,20 +2336,20 @@
       <c r="K20" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="L20" s="29">
+      <c r="L20" s="28">
         <v>0.17</v>
       </c>
       <c r="M20" s="6">
         <v>11</v>
       </c>
-      <c r="N20" s="29">
+      <c r="N20" s="28">
         <f t="shared" si="0"/>
         <v>1.87</v>
       </c>
       <c r="O20" s="6">
         <v>11</v>
       </c>
-      <c r="P20" s="29">
+      <c r="P20" s="28">
         <f t="shared" si="1"/>
         <v>1.87</v>
       </c>
@@ -2385,20 +2382,20 @@
       <c r="K21" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="L21" s="29">
+      <c r="L21" s="28">
         <v>0.1</v>
       </c>
       <c r="M21" s="6">
         <v>1</v>
       </c>
-      <c r="N21" s="29">
+      <c r="N21" s="28">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="O21" s="6">
         <v>1</v>
       </c>
-      <c r="P21" s="29">
+      <c r="P21" s="28">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
@@ -2431,20 +2428,20 @@
       <c r="K22" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="L22" s="29">
+      <c r="L22" s="28">
         <v>0.1</v>
       </c>
       <c r="M22" s="6">
         <v>12</v>
       </c>
-      <c r="N22" s="29">
+      <c r="N22" s="28">
         <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="O22" s="6">
         <v>12</v>
       </c>
-      <c r="P22" s="29">
+      <c r="P22" s="28">
         <f t="shared" si="1"/>
         <v>1.2000000000000002</v>
       </c>
@@ -2477,20 +2474,20 @@
       <c r="K23" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="L23" s="29">
+      <c r="L23" s="28">
         <v>0.1</v>
       </c>
       <c r="M23" s="6">
         <v>1</v>
       </c>
-      <c r="N23" s="29">
+      <c r="N23" s="28">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="O23" s="6">
         <v>1</v>
       </c>
-      <c r="P23" s="29">
+      <c r="P23" s="28">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
@@ -2523,20 +2520,20 @@
       <c r="K24" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="29">
+      <c r="L24" s="28">
         <v>0.1</v>
       </c>
       <c r="M24" s="14">
         <v>16</v>
       </c>
-      <c r="N24" s="29">
+      <c r="N24" s="28">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
       <c r="O24" s="14">
         <v>16</v>
       </c>
-      <c r="P24" s="29">
+      <c r="P24" s="28">
         <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
@@ -2569,20 +2566,20 @@
       <c r="K25" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="L25" s="29">
+      <c r="L25" s="28">
         <v>0.1</v>
       </c>
       <c r="M25" s="6">
         <v>4</v>
       </c>
-      <c r="N25" s="29">
+      <c r="N25" s="28">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="O25" s="6">
         <v>4</v>
       </c>
-      <c r="P25" s="29">
+      <c r="P25" s="28">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
@@ -2615,20 +2612,20 @@
       <c r="K26" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="L26" s="29">
+      <c r="L26" s="28">
         <v>0.3</v>
       </c>
       <c r="M26" s="6">
         <v>2</v>
       </c>
-      <c r="N26" s="29">
+      <c r="N26" s="28">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="O26" s="6">
         <v>2</v>
       </c>
-      <c r="P26" s="29">
+      <c r="P26" s="28">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
@@ -2661,20 +2658,20 @@
       <c r="K27" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="L27" s="29">
+      <c r="L27" s="28">
         <v>35</v>
       </c>
       <c r="M27" s="6">
         <v>1</v>
       </c>
-      <c r="N27" s="29">
+      <c r="N27" s="28">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="O27" s="6">
         <v>1</v>
       </c>
-      <c r="P27" s="29">
+      <c r="P27" s="28">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
@@ -2705,20 +2702,20 @@
       <c r="K28" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="L28" s="29">
+      <c r="L28" s="28">
         <v>3.98</v>
       </c>
       <c r="M28" s="6">
         <v>1</v>
       </c>
-      <c r="N28" s="29">
+      <c r="N28" s="28">
         <f t="shared" si="0"/>
         <v>3.98</v>
       </c>
       <c r="O28" s="6">
         <v>1</v>
       </c>
-      <c r="P28" s="29">
+      <c r="P28" s="28">
         <f t="shared" si="1"/>
         <v>3.98</v>
       </c>
@@ -2751,20 +2748,20 @@
       <c r="K29" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L29" s="29">
+      <c r="L29" s="28">
         <v>0.48</v>
       </c>
       <c r="M29" s="6">
         <v>10</v>
       </c>
-      <c r="N29" s="29">
+      <c r="N29" s="28">
         <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
       <c r="O29" s="6">
         <v>10</v>
       </c>
-      <c r="P29" s="29">
+      <c r="P29" s="28">
         <f t="shared" si="1"/>
         <v>4.8</v>
       </c>
@@ -2797,20 +2794,20 @@
       <c r="K30" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="L30" s="29">
+      <c r="L30" s="28">
         <v>0.87</v>
       </c>
       <c r="M30" s="6">
         <v>4</v>
       </c>
-      <c r="N30" s="29">
+      <c r="N30" s="28">
         <f t="shared" si="0"/>
         <v>3.48</v>
       </c>
       <c r="O30" s="6">
         <v>4</v>
       </c>
-      <c r="P30" s="29">
+      <c r="P30" s="28">
         <f t="shared" si="1"/>
         <v>3.48</v>
       </c>
@@ -2830,23 +2827,23 @@
       <c r="H31" s="23"/>
       <c r="I31" s="9"/>
       <c r="J31" s="8"/>
-      <c r="K31" s="31" t="s">
+      <c r="K31" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="L31" s="29">
+      <c r="L31" s="28">
         <v>0</v>
       </c>
       <c r="M31" s="6">
         <v>1</v>
       </c>
-      <c r="N31" s="29">
+      <c r="N31" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O31" s="6">
         <v>1</v>
       </c>
-      <c r="P31" s="29">
+      <c r="P31" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2857,12 +2854,12 @@
       </c>
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
-      <c r="N32" s="32">
+      <c r="N32" s="31">
         <f>SUM(N4:N31)</f>
         <v>90.416000000000011</v>
       </c>
       <c r="O32" s="19"/>
-      <c r="P32" s="32">
+      <c r="P32" s="31">
         <f>SUM(P4:P31)</f>
         <v>101.536</v>
       </c>

</xml_diff>

<commit_message>
Made change to R4 to reflect part availability.
</commit_message>
<xml_diff>
--- a/LegacyIOBoardBOM.xlsx
+++ b/LegacyIOBoardBOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dedens\Documents\New-Hydra-Legacy-IO-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AFD297-4F30-4B92-B13A-FAAA77704A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDD68ED-07A4-4440-9580-0A0198512B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{E75E0199-A4FC-4142-9D32-2C5EB3346CD5}"/>
+    <workbookView xWindow="-28920" yWindow="-17955" windowWidth="29040" windowHeight="17520" xr2:uid="{E75E0199-A4FC-4142-9D32-2C5EB3346CD5}"/>
   </bookViews>
   <sheets>
     <sheet name="LegacyIOBoard" sheetId="1" r:id="rId1"/>
@@ -470,22 +470,10 @@
     <t>FIXED IND 3.3UH 3A 30 MOHM SMD</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">33.2K </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>33k</t>
-    </r>
-  </si>
-  <si>
     <t>J-1323</t>
+  </si>
+  <si>
+    <t>33k</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1043,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1126,6 +1114,7 @@
     <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="14" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1505,7 +1494,7 @@
   <dimension ref="C3:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2098,7 +2087,7 @@
         <v>43</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>65</v>
@@ -2457,7 +2446,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>47</v>
@@ -2830,20 +2819,20 @@
       <c r="K31" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="L31" s="28">
+      <c r="L31" s="32">
         <v>0</v>
       </c>
-      <c r="M31" s="6">
+      <c r="M31" s="30">
         <v>1</v>
       </c>
-      <c r="N31" s="28">
+      <c r="N31" s="32">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O31" s="6">
+      <c r="O31" s="30">
         <v>1</v>
       </c>
-      <c r="P31" s="28">
+      <c r="P31" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>